<commit_message>
feat: enable enumeration lists in the applicability in combination with specification cardinality "required"
</commit_message>
<xml_diff>
--- a/Excel-files/IDS4ALL-Template.xlsx
+++ b/Excel-files/IDS4ALL-Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5cb7fc635d7635b3/Dokumente/01-Eigene-Dateien/TU-Wien/05-Projekte/2022-AIA4All/IDS/IDS-converter/Excel-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="352" documentId="13_ncr:1_{1B5B4233-0C82-414A-875B-768DAFFA80D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD2CE60C-2FDB-4124-A458-0C34B407AC2D}"/>
+  <xr:revisionPtr revIDLastSave="403" documentId="13_ncr:1_{1B5B4233-0C82-414A-875B-768DAFFA80D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{398CD8C1-E57F-48A8-8FAD-54A8657DDFE8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{16497593-A6A8-4643-B0B9-95B48379E78A}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="290">
   <si>
     <t>IfcLabel</t>
   </si>
@@ -643,9 +643,6 @@
   </si>
   <si>
     <t>SpecificationCardinality</t>
-  </si>
-  <si>
-    <t>required</t>
   </si>
   <si>
     <t>Definition of the cardinality of a specification. The cardinality of a specifcation defines wether the applicable elments must be present in the model. Three different values are valid in this row (required, optional, prohibited). These values are saved in the applicability of a specification and tranformed into the "occurs" attributes of the attribute part of an IDS.
@@ -739,23 +736,6 @@
     <t>Das Dezimaltrennzeichen eines numerischen Werts muss ein Punkt oder ein Komma sein.</t>
   </si>
   <si>
-    <t>Restriction of a numerical value (see 'Example specifications', row 50)</t>
-  </si>
-  <si>
-    <t>Restriction of the number of individual characters of a value (see 'Example specifications', row 49)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Definition of a schema for the character string of the value (see 'Example specifications', row 48). Is defined by regular expressions (regex). </t>
-  </si>
-  <si>
-    <t>This symbol makes it possible to link several values with an 'And' (see 'Example specifications', row 48) . It is used to combine several Facets into one specification. This logic always refers to all columns that belong to a Facet. Care must be taken to ensure that the same number of 'And' symbols are used in all columns of the Facet (e.g. PropertySet: Pset_WallCommon\&amp;Pset_WallCommon; Property: LoadBearing\&amp;Compartmentation; PropertyValue: True\&amp;False). With an optional parameter in IDS, as with PropertyValue, values can also be left blank (e.g. True&amp;). This means that the second value is not defined and the IDS specification specifies that the property must exist with any value.
-Different facets in a line are also merged into one specification. Furthermore, several lines that have the same applicability are also merged into one specification.</t>
-  </si>
-  <si>
-    <t>This symbol seperates values of a 'Or' list within one cell. It is used to define a list of possible values in one cell. The 'Or' symbol has different functionalities in the Requirements and the Applicability. In the Requirements, these values are saved in IDS as a complex ‘enumeration’ restriction (see 'Example specifications', rows 46 and 47).
-In the Applicability, such an enumeration is used to define the Applicability for generally valid values that also apply to specifications with a more specific Applicability (see 'Example specifications', rows 10,11,45) . Therefore, no new specification is created from such a line; instead, the Requirements in this line are added to more specific specifications. Let's have a look on the FireRating definition in the 'Example specifications'. We divide the possible fire resistance values into values for load-bearing walls (REI...) and non-load-bearing walls (EI...) using the LoadBearing property in the Applicability. The general values ND (not defined) and NE (not required) are valid for both categories. To avoid having to include them in both lists, we create a separate list with these two values and define their Applicability for LoadBearing True|False. No separate specification is created here, but these values are added to the specification with the Applicability LoadBearing True and the specification with the Applicability LoadBearing False.</t>
-  </si>
-  <si>
     <t>alle</t>
   </si>
   <si>
@@ -767,13 +747,6 @@
   </si>
   <si>
     <t>Aufbau des Tabellenblattes „Example specifications“</t>
-  </si>
-  <si>
-    <t>The 'Example specifications' sheet introduces individual columns for possible entries in an IDS facet. In a classic or traditional information requirement table there is a column for the IFC entity, defining the applicability, and columns for the property set, property name, property data type and property value to define the requirements. In the same way, columns are introduced for the other IDS facets for both the Applicability and the Requirements. The names of the columns are predefined and must be adhered to. Columns for IDS Applicability start with ‘A.’. Columns for the IDS Requriements start with ‘R.’ Additional general columns (Phase, Role, Usecase, SpecificationCardinality) do not have a prefix. The order of the columns in the Excel table is not predefined. Likewise, not all columns must be present. Columns of IDS facets that are not required can be removed or omitted, which helps to keep the Excel file simple. This makes the IDS4ALL converter applicable to both simple classical information requirements and more elaborate ones using the full potential of IDS. However, if a facet is used, it must be ensured that all required columns of the facet are also used. For example, the ‘PropertySet’ and ‘Property’ entries are required for the Property Facet. If the Property Facet is used, at least these two columns must be filled in.
-The definition of specifications works rowwise. Different rows with the same Applicability are merged into one specification. If the different rows concern different requirements, they are merged with an 'And' logic into one specification. However, different rows often also concern the same requirements, for example, lists of possbile property values are often listen in seperate rows. Therefore, for the columns R.AttributeValue and R.PropertyValue different rows can also be used to list different possible values. If all other entries in the rows are equal, the values in the different rows are merged into one list of possible values with an 'Or' logic (see 'Example specifications', rows 12-21 and 22-31). The second way to define lists of 'Or' values is to use the | delimiter (see description of special characters/symbols).
-The order of the rows is not predefined. Also empty rows are permitted. These are ignored by the converter (see 'Example specifications', rows 54 and 60).
-In general, the row structure is not hierarchical. Each row must be able to stand on its on. This means each row must contain all information and nothing from previous rows is inherited. However, structuring the data by header rows for a new entity or a new property set as in the 'Example specifications' is possible. A header row in the Applicability (see 'Example specifications', row 5) creates an additional general specification, in which all information of the more specific specifications is merged. It does not replace the more specific specifications, it is an additional one. A header row in the Requriements (see 'Example specifications', row 6) does not create a new specification. Instead it is merged with the more detailed specifications below. However, if you separate your data into different IDS files by using the general columns, make sure that the general columns are also filled in for these header rows (should match one of the general data of the more specific specifications below, which one is irrelevant). Otherwise the rows are not merged and incomplete facets are generated.
-Below is a list of the predefined column names divided into Applicability, Requirements and general information, including an explanation:</t>
   </si>
   <si>
     <t>Entity Facet: Definition der IFC-Entität und des PredefinedType in der Form „Entity.PredefinedType“. Wird ein benutzerdefinierter Typ verwendet, muss in dieser Spalte Entity.USERDEFINED und im Attribute Facet über den Objekttyp der benutzerdefinierte Typ definiert werden (siehe „Example specifications“, Zeile 34).</t>
@@ -887,19 +860,10 @@
     <t>Um in einzelnen Zellen mehr als nur einfache Werte zu definieren, sind Schlüsselwörter/-symbole erforderlich. Die Symbole weisen immer auf eine komplexe Einschränkung oder eine spezielle Verarbeitung der Werte in der Zelle hin. Daher sind sie als normaler Text nicht zulässig. Die Symbole sind nicht in jeder Spalte zulässig. Die obige Liste zeigt, welche Symbole in welcher Spalte zulässig sind.</t>
   </si>
   <si>
-    <t>Definition eines Schemas für die Zeichenkette des Wertes (siehe „Example specifications“, Zeile 48). Wird durch reguläre Ausdrücke (regex) definiert.</t>
-  </si>
-  <si>
     <t>Beschränkung der Anzahl der einzelnen Zeichen eines Werts</t>
   </si>
   <si>
-    <t>Beschränkung der Anzahl der einzelnen Zeichen eines Werts (siehe Tabellenblatt 'Example specifications', Zeile 49)</t>
-  </si>
-  <si>
     <t>Beschränkung eines numerischen Werts</t>
-  </si>
-  <si>
-    <t>Beschränkung eines numerischen Werts (see 'Example specifications', row 50)</t>
   </si>
   <si>
     <t>Die Definition verschiedener IFC-Versionen für unterschiedliche Spezifikationen ist nicht möglich. Die angegebene IFC-Version im IDS4ALL-Tabellenblatt wird für jede Spezifikation verwendet.</t>
@@ -994,13 +958,6 @@
     </r>
   </si>
   <si>
-    <t>Das Tabellenblatt „Example specifications“ führt einzelne Spalten für mögliche Einträge in einem IDS Facet ein. In einer klassischen oder traditionellen Informationsanforderungstabelle gibt es eine Spalte für die IFC-Entität, die die Applicability definiert, und Spalten für das PropertySet, den Property-Namen, den Datentyp und den Property-Wert, um die Requirements zu definieren. Auf die gleiche Weise werden Spalten für die anderen IDS Facets sowohl für die Applicability als auch für die Requirements eingeführt. Die Namen der Spalten sind vorgegeben und müssen eingehalten werden. Spalten für die Applicability beginnen mit „A“. Spalten für die Requirements beginnen mit „R“. Zusätzliche allgemeine Spalten (Phase, Role, Usecase, SpecificationCardinality) haben kein Präfix. Die Reihenfolge der Spalten in der Excel-Tabelle ist nicht vorgegeben. Ebenso müssen nicht alle Spalten vorhanden sein. Spalten von IDS Facets, die nicht erforderlich sind, können entfernt oder weggelassen werden, wodurch die Excel-Datei einfach gehalten werden kann. Dadurch kann der IDS4ALL-Konverter sowohl für einfache klassische Informationsanforderungen als auch für komplexere Anforderungen verwendet werden, die das volle Potenzial von IDS nutzen. Wenn ein Facet verwendet wird, muss jedoch sichergestellt werden, dass auch alle erforderlichen Spalten des Facets verwendet werden. Beispielsweise sind die Einträge „PropertySet“ und „Property“ für das Property Facet erforderlich. Wenn das Property Facet verwendet wird, müssen mindestens diese beiden Spalten ausgefüllt werden.
-Die Definition von Spezifikationen erfolgt zeilenweise. Verschiedene Zeilen mit der gleichen Applicability werden zu einer Spezifikation zusammengefasst. Wenn die verschiedenen Zeilen unterschiedliche Requirements betreffen, werden sie mit einer „Und“-Logik zu einer Spezifikation zusammengefasst. Verschiedene Zeilen betreffen jedoch oft auch dieselben Requirements, z. B. werden Listen möglicher Eigenschaftswerte oft in separaten Zeilen aufgeführt. Daher können für die Spalten R.AttributeValue und R.PropertyValue auch verschiedene Zeilen verwendet werden, um verschiedene mögliche Werte aufzulisten. Wenn alle anderen Einträge in den Zeilen gleich sind, werden die Werte in den verschiedenen Zeilen mit einer „Oder“-Logik zu einer Liste möglicher Werte zusammengeführt (siehe „Example specifications“, Zeilen 12–21 und 22–31). Die zweite Möglichkeit, Listen von „Oder“-Werten zu definieren, ist die Verwendung des Trennzeichens | (siehe Beschreibung der Schlüsselwörter/-symbole).
-Die Reihenfolge der Zeilen ist nicht vorgegeben. Auch leere Zeilen sind zulässig. Diese werden vom Konverter ignoriert (siehe „Example specifications“, Zeilen 54 und 60).
-Im Allgemeinen ist die Zeilenstruktur nicht hierarchisch. Jede Zeile muss für sich allein stehen können. Das bedeutet, dass jede Zeile alle Informationen enthalten muss und keine Informationen aus vorherigen Zeilen übernommen werden. Es ist jedoch möglich, die Daten durch Überschriftszeilen für eine neue Entität oder ein neues PropertySet wie in den „Example specifications“ zu strukturieren. Eine Überschriftszeile in der Applicability (siehe „Example specifications“, Zeile 5) erstellt eine zusätzliche allgemeine Spezifikation, in der alle Informationen der spezifischeren Spezifikationen zusammengeführt werden. Sie ersetzt nicht die spezifischeren Spezifikation, sondern ist eine zusätzliche Spezifikation. Eine Überschirftszeile in den Requirements (siehe „Example specifications“, Zeile 6) erstellt keine neue Spezifikation. Stattdessen wird sie mit den detaillierteren Spezifikationen darunter zusammengeführt. Wenn Sie Ihre Daten jedoch mithilfe der allgemeinen Spalten in verschiedene IDS-Dateien aufteilen, stellen Sie sicher, dass die allgemeinen Spalten auch für diese Überschriftszeilen ausgefüllt werden (sollten mit den allgemeinen Daten einer spezifischeren Spezifikation übereinstimmen, wobei es unerheblich ist, mit welcher spezifischeren Spezifikation). Andernfalls werden die Zeilen nicht zusammengeführt und es werden unvollständige Facets generiert.
-Nachfolgend finden Sie eine Liste der vordefinierten Spaltennamen, unterteilt in Applicability, Requirements und allgemeine Informationen, einschließlich einer Erklärung:</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Entity Facet: Beschreibung der IFC-Entität. Kann in Kombination mit dem Entity Facet in den Anforderungen verwendet werden, um allgemeine Informationen über eine Entität in den Instructions des Entity Facet zu speichern. Wird beispielsweise verwendet, um eine eindeutige Beschreibung aller Entitäten bereitzustellen, die in den Informationsanforderungen erscheinen. Zu diesem Zweck kann eine Spezifikation das Entity Facet in der Applicability und in den Requirements enthalten, wobei in den Requirements die Beschreibung hinzugefügt wird. (siehe „Example specifications“, Zeilen 3 und 4). Eine Beschreibung ist nur in den Requirements möglich, da das IDS-Schema keine </t>
     </r>
@@ -1081,14 +1038,6 @@
 Standardmäßig ist die Kardinalität der Spezifikationen optional, wenn die Spalte nicht verwendet wird.</t>
   </si>
   <si>
-    <t>Dieses Symbol trennt die Werte einer „Oder“-Liste innerhalb einer Zelle. Es wird verwendet, um eine Liste möglicher Werte in einer Zelle zu definieren. Das „Oder“-Symbol hat in den Requirements und in der Applicability unterschiedliche Funktionen. In den Requirements werden diese Werte in IDS als komplexe „Aufzählungs“-Einschränkung gespeichert (siehe „Example specifications“, Zeilen 46 und 47).
-In der Applicability wird eine solche Aufzählung verwendet, um die Applicability für allgemein gültige Werte zu definieren, die auch für Spezifikationen mit einer spezifischeren Applicability gelten (siehe „Example specifications“, Zeilen 10, 11, 45). Daher wird aus einer solchen Zeile keine neue Spezifikation erstellt; stattdessen werden die Requirements in dieser Zeile zu spezifischeren Spezifikationen hinzugefügt. Sehen wir uns die Definition von FireRating in den „Example specifications“ an. Wir unterteilen die möglichen Feuerwiderstandswerte in Werte für tragende Wände (REI...) und nicht tragende Wände (EI...) unter Verwendung der Eigenschaft LoadBearing in der Applicability. Die allgemeinen Werte ND (nicht definiert) und NE (nicht erforderlich) gelten für beide Kategorien. Um zu vermeiden, dass sie in beide Listen aufgenommen werden müssen, erstellen wir eine separate Liste mit diesen beiden Werten und definieren ihre Applicability für LoadBearing True|False. Hier wird keine separate Spezifikation erstellt, sondern diese Werte werden der Spezifikation mit der Applicability LoadBearing True und der Spezifikation mit der Applicability LoadBearing False hinzugefügt.</t>
-  </si>
-  <si>
-    <t>Dieses Symbol ermöglicht es, mehrere Werte mit einem „Und“ zu verknüpfen (siehe „Example specifications“, Zeile 48). Es wird verwendet, um mehrere Facets in einer Spezifikation zu kombinieren. Diese Logik bezieht sich immer auf alle Spalten, die zu einem Facet gehören. Es muss darauf geachtet werden, dass in allen Spalten des Facets die gleiche Anzahl von „Und“-Symbolen verwendet wird (z. B. PropertySet: Pset_WallCommon\&amp;Pset_WallCommon; Property: LoadBearing\&amp;Compartmentation; PropertyValue: True\&amp;False). Bei einem optionalen Parameter in IDS wie bei PropertyValue können Werte auch leer gelassen werden (z. B. True&amp;). Dies bedeutet, dass der zweite Wert nicht definiert ist und die IDS-Spezifikation angibt, dass die Eigenschaft mit einem beliebigen Wert vorhanden sein muss.
-Verschiedene Facets in einer Zeile werden ebenfalls zu einer Spezifikation zusammengeführt. Darüber hinaus werden auch mehrere Zeilen mit derselben Applicability zu einer Spezifikation zusammengeführt.</t>
-  </si>
-  <si>
     <t>kleiner gleich</t>
   </si>
   <si>
@@ -1099,12 +1048,6 @@
   </si>
   <si>
     <t>größer gleich</t>
-  </si>
-  <si>
-    <t>Das Erstellen von „Aufzählungs“-Listen in der Applicability ist nicht möglich. Da das „Oder“-Symbol verwendet wird, um eine allgemeine Applicability zu definieren, werden durch | getrennte Werte in andere spezifischere Spezifikationen aufgenommen, anstatt eine neue Spezifikation mit einer komplexen Aufzählung in der Applicability zu erstellen.</t>
-  </si>
-  <si>
-    <t>Generating 'enumerations' restrictions in the applicability is not possible. Since the 'Or' symbol is used to define a general applicability, values seperated by | are included in other more specific specifiactions instead of creating a new specification with a complex enumeration in the applicability.</t>
   </si>
   <si>
     <t>This IDS4ALL converter, developed by Simon Fischer, Harald Urban, Konstantin Höbart and Christian Schranz from the Digital Building Process research group at the TU Wien (https://www.tuwien.at/cee/ibb/zdb), transfers information requirements from an Excel file into an IDS file. In practice, information requirements are often defined in tabular form in Excel. This tool is designed to help you easily transfer them to IDS while taking advantage of the full functionality of IDS. The aim is to use an Excel file structure that is similar to the existing structures for information requirements in order to facilitate the adaptation to IDS.
@@ -1198,6 +1141,59 @@
       </rPr>
       <t>, these values are ignored in the merge process. Enumerations are merged into one requirement.</t>
     </r>
+  </si>
+  <si>
+    <t>IfcRelSpaceBoundary|IfcRelSpaceBoundary2ndLevel</t>
+  </si>
+  <si>
+    <t>Das Tabellenblatt „Example specifications“ führt einzelne Spalten für mögliche Einträge in einem IDS Facet ein. In einer klassischen oder traditionellen Informationsanforderungstabelle gibt es eine Spalte für die IFC-Entität, die die Applicability definiert, und Spalten für das PropertySet, den Property-Namen, den Datentyp und den Property-Wert, um die Requirements zu definieren. Auf die gleiche Weise werden Spalten für die anderen IDS Facets sowohl für die Applicability als auch für die Requirements eingeführt. Die Namen der Spalten sind vorgegeben und müssen eingehalten werden. Spalten für die Applicability beginnen mit „A“. Spalten für die Requirements beginnen mit „R“. Zusätzliche allgemeine Spalten (Phase, Role, Usecase, SpecificationCardinality) haben kein Präfix. Die Reihenfolge der Spalten in der Excel-Tabelle ist nicht vorgegeben. Ebenso müssen nicht alle Spalten vorhanden sein. Spalten von IDS Facets, die nicht erforderlich sind, können entfernt oder weggelassen werden, wodurch die Excel-Datei einfach gehalten werden kann. Dadurch kann der IDS4ALL-Konverter sowohl für einfache klassische Informationsanforderungen als auch für komplexere Anforderungen verwendet werden, die das volle Potenzial von IDS nutzen. Wenn ein Facet verwendet wird, muss jedoch sichergestellt werden, dass auch alle erforderlichen Spalten des Facets verwendet werden. Beispielsweise sind die Einträge „PropertySet“ und „Property“ für das Property Facet erforderlich. Wenn das Property Facet verwendet wird, müssen mindestens diese beiden Spalten ausgefüllt werden.
+Die Definition von Spezifikationen erfolgt zeilenweise. Verschiedene Zeilen mit der gleichen Applicability werden zu einer Spezifikation zusammengefasst. Wenn die verschiedenen Zeilen unterschiedliche Requirements betreffen, werden sie mit einer „Und“-Logik zu einer Spezifikation zusammengefasst. Verschiedene Zeilen betreffen jedoch oft auch dieselben Requirements, z. B. werden Listen möglicher Eigenschaftswerte oft in separaten Zeilen aufgeführt. Daher können für die Spalten R.AttributeValue und R.PropertyValue auch verschiedene Zeilen verwendet werden, um verschiedene mögliche Werte aufzulisten. Wenn alle anderen Einträge in den Zeilen gleich sind, werden die Werte in den verschiedenen Zeilen mit einer „Oder“-Logik zu einer Liste möglicher Werte zusammengeführt (siehe „Example specifications“, Zeilen 12–21 und 22–31). Die zweite Möglichkeit, Listen von „Oder“-Werten zu definieren, ist die Verwendung des Trennzeichens | (siehe Beschreibung der Schlüsselwörter/-symbole).
+Die Reihenfolge der Zeilen ist nicht vorgegeben. Auch leere Zeilen sind zulässig. Diese werden vom Konverter ignoriert (siehe „Example specifications“, Zeilen 55 und 61).
+Im Allgemeinen ist die Zeilenstruktur nicht hierarchisch. Jede Zeile muss für sich allein stehen können. Das bedeutet, dass jede Zeile alle Informationen enthalten muss und keine Informationen aus vorherigen Zeilen übernommen werden. Es ist jedoch möglich, die Daten durch Überschriftszeilen für eine neue Entität oder ein neues PropertySet wie in den „Example specifications“ zu strukturieren. Eine Überschriftszeile in der Applicability (siehe „Example specifications“, Zeile 5) erstellt eine zusätzliche allgemeine Spezifikation, in der alle Informationen der spezifischeren Spezifikationen zusammengeführt werden. Sie ersetzt nicht die spezifischeren Spezifikation, sondern ist eine zusätzliche Spezifikation. Eine Überschirftszeile in den Requirements (siehe „Example specifications“, Zeile 6) erstellt keine neue Spezifikation. Stattdessen wird sie mit den detaillierteren Spezifikationen darunter zusammengeführt. Wenn Sie Ihre Daten jedoch mithilfe der allgemeinen Spalten in verschiedene IDS-Dateien aufteilen, stellen Sie sicher, dass die allgemeinen Spalten auch für diese Überschriftszeilen ausgefüllt werden (sollten mit den allgemeinen Daten einer spezifischeren Spezifikation übereinstimmen, wobei es unerheblich ist, mit welcher spezifischeren Spezifikation). Andernfalls werden die Zeilen nicht zusammengeführt und es werden unvollständige Facets generiert.
+Nachfolgend finden Sie eine Liste der vordefinierten Spaltennamen, unterteilt in Applicability, Requirements und allgemeine Informationen, einschließlich einer Erklärung:</t>
+  </si>
+  <si>
+    <t>The 'Example specifications' sheet introduces individual columns for possible entries in an IDS facet. In a classic or traditional information requirement table there is a column for the IFC entity, defining the applicability, and columns for the property set, property name, property data type and property value to define the requirements. In the same way, columns are introduced for the other IDS facets for both the Applicability and the Requirements. The names of the columns are predefined and must be adhered to. Columns for IDS Applicability start with ‘A.’. Columns for the IDS Requriements start with ‘R.’ Additional general columns (Phase, Role, Usecase, SpecificationCardinality) do not have a prefix. The order of the columns in the Excel table is not predefined. Likewise, not all columns must be present. Columns of IDS facets that are not required can be removed or omitted, which helps to keep the Excel file simple. This makes the IDS4ALL converter applicable to both simple classical information requirements and more elaborate ones using the full potential of IDS. However, if a facet is used, it must be ensured that all required columns of the facet are also used. For example, the ‘PropertySet’ and ‘Property’ entries are required for the Property Facet. If the Property Facet is used, at least these two columns must be filled in.
+The definition of specifications works rowwise. Different rows with the same Applicability are merged into one specification. If the different rows concern different requirements, they are merged with an 'And' logic into one specification. However, different rows often also concern the same requirements, for example, lists of possbile property values are often listen in seperate rows. Therefore, for the columns R.AttributeValue and R.PropertyValue different rows can also be used to list different possible values. If all other entries in the rows are equal, the values in the different rows are merged into one list of possible values with an 'Or' logic (see 'Example specifications', rows 12-21 and 22-31). The second way to define lists of 'Or' values is to use the | delimiter (see description of special characters/symbols).
+The order of the rows is not predefined. Also empty rows are permitted. These are ignored by the converter (see 'Example specifications', rows 55 and 61).
+In general, the row structure is not hierarchical. Each row must be able to stand on its on. This means each row must contain all information and nothing from previous rows is inherited. However, structuring the data by header rows for a new entity or a new property set as in the 'Example specifications' is possible. A header row in the Applicability (see 'Example specifications', row 5) creates an additional general specification, in which all information of the more specific specifications is merged. It does not replace the more specific specifications, it is an additional one. A header row in the Requriements (see 'Example specifications', row 6) does not create a new specification. Instead it is merged with the more detailed specifications below. However, if you separate your data into different IDS files by using the general columns, make sure that the general columns are also filled in for these header rows (should match one of the general data of the more specific specifications below, which one is irrelevant). Otherwise the rows are not merged and incomplete facets are generated.
+Below is a list of the predefined column names divided into Applicability, Requirements and general information, including an explanation:</t>
+  </si>
+  <si>
+    <t>Dieses Symbol trennt die Werte einer „Oder“-Liste innerhalb einer Zelle. Es wird verwendet, um eine Liste möglicher Werte in einer Zelle zu definieren. Das „Oder“-Symbol hat in den Requirements und in der Applicability unterschiedliche Funktionen. In den Requirements werden diese Werte in IDS als komplexe „Aufzählungs“-Einschränkung gespeichert (siehe „Example specifications“, Zeilen 47 und 48).
+In der Applicability wird eine solche Aufzählung verwendet, um mehrere Elemente zu beschreiben für die eine Anforderung gilt. Dies ist sehr gut geeignet, um die Applicability für allgemein gültige Werte zu definieren, die auch für Spezifikationen mit einer spezifischeren Applicability gelten (siehe „Example specifications“, Zeilen 10, 11, 46). Um die spezifischeren Werte zu den allgemeinen Werten hinzufügen zu können, wird eine solche Zeile in mehrere Spezifikationen aufgeteilt, je eine für die unterschiedlichen "Oder"-Werte. Dadurch entstehen aus der allgemeinen Spezifikation bereits Spezifikationen mit spezifischer Applicability, die mit den späteren spezifischen Spezifikationen vereint werden können. Sehen wir uns die Definition von FireRating in den „Example specifications“ an. Wir unterteilen die möglichen Feuerwiderstandswerte in Werte für tragende Wände (REI...) und nicht tragende Wände (EI...) unter Verwendung der Eigenschaft LoadBearing in der Applicability. Die allgemeinen Werte ND (nicht definiert) und NE (nicht erforderlich) gelten für beide Kategorien. Um zu vermeiden, dass sie in beide Listen aufgenommen werden müssen, erstellen wir eine separate Liste mit diesen beiden Werten und definieren ihre Applicability für LoadBearing True|False. Diese beiden "Oder"-Werte werden in zwei einzelne Spezifiaktionen aufgeteilt, einmal für LoadBearing True und einmal für LoadBearing false, jeweils mit den FireRating-Werten ND|NE. Die nächsten Zeilen haben anschleißend die gleiche Applicability wie eine der bereits vorhandenen Spezifikationen und können vereinigt werden. Es resultieren zwei verschiedene Spezifikationen.
+Eine Ausnahme bildet die Verwendung der SpecificationCardinality "Required". Wird mithilfe dieser Funktion die Existenz von Elementen im Modell gefordert, können die "Oder"-Werte nicht in einzelne Spezifikationen aufgeteilt werden, da dadurch die Logik verloren geht, dass nur eines der definierten Elemente im Modell enthalten sein muss. VORSICHT: Daher können spezifische und allgemeine Werte in Kombination mit SpecificationCardinality "Required" nicht zusammengefügt werden und unvollständige Auswahllisten können entstehen.</t>
+  </si>
+  <si>
+    <t>This symbol makes it possible to link several values with an 'And' (see 'Example specifications', row 49) . It is used to combine several Facets into one specification. This logic always refers to all columns that belong to a Facet. Care must be taken to ensure that the same number of 'And' symbols are used in all columns of the Facet (e.g. PropertySet: Pset_WallCommon\&amp;Pset_WallCommon; Property: LoadBearing\&amp;Compartmentation; PropertyValue: True\&amp;False). With an optional parameter in IDS, as with PropertyValue, values can also be left blank (e.g. True&amp;). This means that the second value is not defined and the IDS specification specifies that the property must exist with any value.
+Different facets in a line are also merged into one specification. Furthermore, several lines that have the same applicability are also merged into one specification.</t>
+  </si>
+  <si>
+    <t>Dieses Symbol ermöglicht es, mehrere Werte mit einem „Und“ zu verknüpfen (siehe „Example specifications“, Zeile 49). Es wird verwendet, um mehrere Facets in einer Spezifikation zu kombinieren. Diese Logik bezieht sich immer auf alle Spalten, die zu einem Facet gehören. Es muss darauf geachtet werden, dass in allen Spalten des Facets die gleiche Anzahl von „Und“-Symbolen verwendet wird (z. B. PropertySet: Pset_WallCommon\&amp;Pset_WallCommon; Property: LoadBearing\&amp;Compartmentation; PropertyValue: True\&amp;False). Bei einem optionalen Parameter in IDS wie bei PropertyValue können Werte auch leer gelassen werden (z. B. True&amp;). Dies bedeutet, dass der zweite Wert nicht definiert ist und die IDS-Spezifikation angibt, dass die Eigenschaft mit einem beliebigen Wert vorhanden sein muss.
+Verschiedene Facets in einer Zeile werden ebenfalls zu einer Spezifikation zusammengeführt. Darüber hinaus werden auch mehrere Zeilen mit derselben Applicability zu einer Spezifikation zusammengeführt.</t>
+  </si>
+  <si>
+    <t>Definition eines Schemas für die Zeichenkette des Wertes (siehe „Example specifications“, Zeile 49). Wird durch reguläre Ausdrücke (regex) definiert.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definition of a schema for the character string of the value (see 'Example specifications', row 49). Is defined by regular expressions (regex). </t>
+  </si>
+  <si>
+    <t>Beschränkung der Anzahl der einzelnen Zeichen eines Werts (siehe Tabellenblatt 'Example specifications', Zeile 50)</t>
+  </si>
+  <si>
+    <t>Beschränkung eines numerischen Werts (see 'Example specifications', row 51)</t>
+  </si>
+  <si>
+    <t>Restriction of the number of individual characters of a value (see 'Example specifications', row 50)</t>
+  </si>
+  <si>
+    <t>Restriction of a numerical value (see 'Example specifications', row 51)</t>
+  </si>
+  <si>
+    <t>This symbol seperates values of a 'Or' list within one cell. It is used to define a list of possible values in one cell. The 'Or' symbol has different functionalities in the Requirements and the Applicability. In the Requirements, these values are saved in IDS as a complex ‘enumeration’ restriction (see 'Example specifications', rows 47 and 48).
+In Applicability, such a list is used to describe multiple elements to which a requirement applies. This is very well suited for defining the applicability for generally valid values that also apply to specifications with a more specific applicability (see ‘Example specifications’, lines 10, 11, 46). In order to add the more specific values to the general values, such a line is divided into several specifications, one for each of the different ‘Or’ values. This results in specifications with specific applicability, which can be combined with the later specific specifications. Let's look at the definition of FireRating in the ‘Example specifications’. We divide the possible fire resistance values into values for load-bearing walls (REI...) and non-load-bearing walls (EI...) using the LoadBearing property in the Applicability. The general values ND (not defined) and NE (not required) apply to both categories. To avoid having to include them in both lists, we create a separate list with these two values and define their Applicability for LoadBearing as True|False. These two ‘Or’ values are split into two individual specifications, one for LoadBearing True and one for LoadBearing false, each with the FireRating values ND|NE. The next lines then have the same applicability as one of the existing specifications and can be merged. This results in two different specifications.
+An exception is the use of the SpecificationCardinality ‘Required’. If this function is used to require the existence of elements in the model, the ‘Or’ values cannot be split into individual specifications, as this would lose the logic that only one of the defined elements must be contained in the model. CAUTION: Therefore, specific and general values cannot be combined when SpecificationCardinality ‘Required’ is defined and incomplete selection lists may result.</t>
   </si>
 </sst>
 </file>
@@ -2540,7 +2536,7 @@
         <v>71</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>72</v>
@@ -2570,7 +2566,7 @@
         <v>75</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>72</v>
@@ -2641,7 +2637,7 @@
         <v>80</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>72</v>
@@ -2670,17 +2666,17 @@
     </row>
     <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="60" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="17" t="s">
         <v>74</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2793,7 +2789,7 @@
         <v>50</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>51</v>
@@ -2871,7 +2867,7 @@
         <v>122</v>
       </c>
       <c r="AD2" s="4" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>19</v>
@@ -3108,10 +3104,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134D532F-CD5A-45F4-AF33-42136DA547E7}">
-  <dimension ref="A1:AJ165"/>
+  <dimension ref="A1:AJ166"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A50" sqref="A50:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3202,7 +3198,7 @@
         <v>50</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>51</v>
@@ -3280,7 +3276,7 @@
         <v>122</v>
       </c>
       <c r="AD2" s="4" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>19</v>
@@ -3408,7 +3404,7 @@
         <v>171</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>201</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:36" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3442,7 +3438,7 @@
         <v>171</v>
       </c>
       <c r="AH6" s="13" t="s">
-        <v>201</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
@@ -3484,7 +3480,7 @@
         <v>171</v>
       </c>
       <c r="AH7" s="5" t="s">
-        <v>201</v>
+        <v>72</v>
       </c>
       <c r="AI7" s="5"/>
       <c r="AJ7" s="5"/>
@@ -3526,7 +3522,7 @@
         <v>171</v>
       </c>
       <c r="AH8" s="5" t="s">
-        <v>201</v>
+        <v>72</v>
       </c>
       <c r="AI8" s="5"/>
       <c r="AJ8" s="5"/>
@@ -3618,6 +3614,7 @@
       <c r="AG10" s="5" t="s">
         <v>171</v>
       </c>
+      <c r="AH10" s="5"/>
       <c r="AI10" s="5"/>
       <c r="AJ10" s="5"/>
     </row>
@@ -3667,6 +3664,7 @@
       <c r="AG11" s="5" t="s">
         <v>171</v>
       </c>
+      <c r="AH11" s="5"/>
       <c r="AI11" s="5"/>
       <c r="AJ11" s="5"/>
     </row>
@@ -4917,7 +4915,7 @@
       </c>
       <c r="V38" s="8"/>
       <c r="AD38" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="AE38" s="5" t="s">
         <v>168</v>
@@ -4957,7 +4955,7 @@
       </c>
       <c r="V39" s="8"/>
       <c r="AD39" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="AE39" s="5" t="s">
         <v>168</v>
@@ -4973,17 +4971,17 @@
     </row>
     <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
@@ -5000,142 +4998,131 @@
       <c r="AF40" s="5"/>
       <c r="AG40" s="5"/>
       <c r="AH40" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AI40" s="5"/>
       <c r="AJ40" s="5"/>
     </row>
-    <row r="41" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+      <c r="V41" s="8"/>
+      <c r="AE41" s="5"/>
+      <c r="AF41" s="5"/>
+      <c r="AG41" s="5"/>
+      <c r="AH41" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI41" s="5"/>
+      <c r="AJ41" s="5"/>
+    </row>
+    <row r="42" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
-      <c r="O41" s="14"/>
-      <c r="AE41" s="1" t="s">
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14"/>
+      <c r="AE42" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="AF41" s="1" t="s">
+      <c r="AF42" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AG41" s="1" t="s">
+      <c r="AG42" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="AI41" s="14"/>
-      <c r="AJ41" s="14"/>
-    </row>
-    <row r="42" spans="1:36" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
+      <c r="AI42" s="14"/>
+      <c r="AJ42" s="14"/>
+    </row>
+    <row r="43" spans="1:36" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="13"/>
-      <c r="K42" s="13"/>
-      <c r="L42" s="13"/>
-      <c r="M42" s="11" t="s">
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="N42" s="13"/>
-      <c r="O42" s="13"/>
-      <c r="AE42" s="12" t="s">
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
+      <c r="AE43" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="AF42" s="12" t="s">
+      <c r="AF43" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="AG42" s="12" t="s">
+      <c r="AG43" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="AI42" s="13"/>
-      <c r="AJ42" s="13"/>
-    </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="5"/>
-      <c r="M43" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="N43" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="O43" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="S43" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="T43" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="AE43" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="AF43" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="AG43" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="AI43" s="5"/>
-      <c r="AJ43" s="5"/>
+      <c r="AI43" s="13"/>
+      <c r="AJ43" s="13"/>
     </row>
     <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="7"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
       <c r="M44" s="5" t="s">
         <v>33</v>
       </c>
       <c r="N44" s="5" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
       <c r="O44" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="P44" s="7"/>
-      <c r="Q44" s="7"/>
-      <c r="R44" s="7"/>
+      <c r="S44" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="T44" s="5" t="s">
+        <v>192</v>
+      </c>
       <c r="AE44" s="5" t="s">
         <v>167</v>
       </c>
@@ -5145,42 +5132,36 @@
       <c r="AG44" s="5" t="s">
         <v>171</v>
       </c>
+      <c r="AI44" s="5"/>
+      <c r="AJ44" s="5"/>
     </row>
     <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
       <c r="M45" s="5" t="s">
         <v>33</v>
       </c>
       <c r="N45" s="5" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="O45" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="P45" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q45" s="5"/>
-      <c r="R45" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="P45" s="7"/>
+      <c r="Q45" s="7"/>
+      <c r="R45" s="7"/>
       <c r="AE45" s="5" t="s">
         <v>167</v>
       </c>
@@ -5203,7 +5184,7 @@
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
@@ -5221,9 +5202,8 @@
       <c r="O46" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="P46" s="5" t="str">
-        <f>_xlfn.TEXTJOIN("|",TRUE,P12:P21)</f>
-        <v>EI 30|EI 60|EI 90|EI 120|EI 180|E 30|E 60|E 90|E 120|E 180</v>
+      <c r="P46" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="Q46" s="5"/>
       <c r="R46" s="5"/>
@@ -5249,7 +5229,7 @@
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="5" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
@@ -5268,8 +5248,8 @@
         <v>0</v>
       </c>
       <c r="P47" s="5" t="str">
-        <f>_xlfn.TEXTJOIN("|",TRUE,P22:P31)</f>
-        <v>R 30|R 60|R 90|R 120|R 180|REI 30|REI 60|REI 90|REI 120|REI 180</v>
+        <f>_xlfn.TEXTJOIN("|",TRUE,P12:P21)</f>
+        <v>EI 30|EI 60|EI 90|EI 120|EI 180|E 30|E 60|E 90|E 120|E 180</v>
       </c>
       <c r="Q47" s="5"/>
       <c r="R47" s="5"/>
@@ -5288,14 +5268,14 @@
         <v>87</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>183</v>
+        <v>33</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>184</v>
+        <v>4</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5" t="s">
-        <v>185</v>
+        <v>7</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
@@ -5313,8 +5293,9 @@
       <c r="O48" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="P48" s="5" t="s">
-        <v>34</v>
+      <c r="P48" s="5" t="str">
+        <f>_xlfn.TEXTJOIN("|",TRUE,P22:P31)</f>
+        <v>R 30|R 60|R 90|R 120|R 180|REI 30|REI 60|REI 90|REI 120|REI 180</v>
       </c>
       <c r="Q48" s="5"/>
       <c r="R48" s="5"/>
@@ -5332,10 +5313,16 @@
       <c r="A49" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
+      <c r="B49" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>184</v>
+      </c>
       <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
+      <c r="E49" s="5" t="s">
+        <v>185</v>
+      </c>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
@@ -5347,13 +5334,13 @@
         <v>33</v>
       </c>
       <c r="N49" s="5" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="O49" s="5" t="s">
         <v>0</v>
       </c>
       <c r="P49" s="5" t="s">
-        <v>186</v>
+        <v>34</v>
       </c>
       <c r="Q49" s="5"/>
       <c r="R49" s="5"/>
@@ -5386,13 +5373,13 @@
         <v>33</v>
       </c>
       <c r="N50" s="5" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="O50" s="5" t="s">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="P50" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Q50" s="5"/>
       <c r="R50" s="5"/>
@@ -5425,12 +5412,14 @@
         <v>33</v>
       </c>
       <c r="N51" s="5" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="O51" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="P51" s="5"/>
+        <v>86</v>
+      </c>
+      <c r="P51" s="5" t="s">
+        <v>187</v>
+      </c>
       <c r="Q51" s="5"/>
       <c r="R51" s="5"/>
       <c r="AE51" s="5" t="s">
@@ -5462,10 +5451,10 @@
         <v>33</v>
       </c>
       <c r="N52" s="5" t="s">
-        <v>84</v>
+        <v>6</v>
       </c>
       <c r="O52" s="5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P52" s="5"/>
       <c r="Q52" s="5"/>
@@ -5499,10 +5488,10 @@
         <v>33</v>
       </c>
       <c r="N53" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O53" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P53" s="5"/>
       <c r="Q53" s="5"/>
@@ -5518,7 +5507,9 @@
       </c>
     </row>
     <row r="54" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
+      <c r="A54" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
@@ -5530,20 +5521,30 @@
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
-      <c r="M54" s="5"/>
-      <c r="N54" s="5"/>
-      <c r="O54" s="5"/>
+      <c r="M54" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N54" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="O54" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="P54" s="5"/>
       <c r="Q54" s="5"/>
       <c r="R54" s="5"/>
-      <c r="AE54" s="5"/>
-      <c r="AF54" s="5"/>
-      <c r="AG54" s="5"/>
+      <c r="AE54" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="AF54" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="AG54" s="5" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="55" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
@@ -5551,37 +5552,19 @@
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
-      <c r="I55" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="J55" s="5" t="s">
-        <v>97</v>
-      </c>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
-      <c r="M55" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="N55" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="O55" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="P55" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="M55" s="5"/>
+      <c r="N55" s="5"/>
+      <c r="O55" s="5"/>
+      <c r="P55" s="5"/>
       <c r="Q55" s="5"/>
       <c r="R55" s="5"/>
-      <c r="AE55" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="AF55" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="AG55" s="5" t="s">
-        <v>171</v>
-      </c>
+      <c r="AE55" s="5"/>
+      <c r="AF55" s="5"/>
+      <c r="AG55" s="5"/>
     </row>
     <row r="56" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
@@ -5606,13 +5589,13 @@
         <v>3</v>
       </c>
       <c r="N56" s="5" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
       <c r="O56" s="5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P56" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="Q56" s="5"/>
       <c r="R56" s="5"/>
@@ -5649,13 +5632,13 @@
         <v>3</v>
       </c>
       <c r="N57" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O57" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P57" s="5" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="Q57" s="5"/>
       <c r="R57" s="5"/>
@@ -5692,7 +5675,7 @@
         <v>3</v>
       </c>
       <c r="N58" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O58" s="5" t="s">
         <v>1</v>
@@ -5735,13 +5718,13 @@
         <v>3</v>
       </c>
       <c r="N59" s="5" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="O59" s="5" t="s">
-        <v>86</v>
+        <v>1</v>
       </c>
       <c r="P59" s="5" t="s">
-        <v>98</v>
+        <v>7</v>
       </c>
       <c r="Q59" s="5"/>
       <c r="R59" s="5"/>
@@ -5756,7 +5739,9 @@
       </c>
     </row>
     <row r="60" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
+      <c r="A60" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
@@ -5764,24 +5749,40 @@
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
-      <c r="J60" s="5"/>
+      <c r="I60" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
-      <c r="M60" s="5"/>
-      <c r="N60" s="5"/>
-      <c r="O60" s="5"/>
-      <c r="P60" s="5"/>
+      <c r="M60" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="N60" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O60" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="P60" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="Q60" s="5"/>
       <c r="R60" s="5"/>
-      <c r="AE60" s="5"/>
-      <c r="AF60" s="5"/>
-      <c r="AG60" s="5"/>
+      <c r="AE60" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="AF60" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="AG60" s="5" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="61" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="A61" s="5"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
@@ -5789,37 +5790,19 @@
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
-      <c r="I61" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="J61" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
-      <c r="M61" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="N61" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="O61" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="P61" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="M61" s="5"/>
+      <c r="N61" s="5"/>
+      <c r="O61" s="5"/>
+      <c r="P61" s="5"/>
       <c r="Q61" s="5"/>
       <c r="R61" s="5"/>
-      <c r="AE61" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="AF61" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="AG61" s="5" t="s">
-        <v>171</v>
-      </c>
+      <c r="AE61" s="5"/>
+      <c r="AF61" s="5"/>
+      <c r="AG61" s="5"/>
     </row>
     <row r="62" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
@@ -5844,13 +5827,13 @@
         <v>3</v>
       </c>
       <c r="N62" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O62" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P62" s="5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Q62" s="5"/>
       <c r="R62" s="5"/>
@@ -5865,7 +5848,9 @@
       </c>
     </row>
     <row r="63" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A63" s="5"/>
+      <c r="A63" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
@@ -5873,19 +5858,37 @@
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
-      <c r="J63" s="5"/>
+      <c r="I63" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
-      <c r="M63" s="5"/>
-      <c r="N63" s="5"/>
-      <c r="O63" s="5"/>
-      <c r="P63" s="5"/>
+      <c r="M63" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="N63" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O63" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P63" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="Q63" s="5"/>
       <c r="R63" s="5"/>
-      <c r="AE63" s="5"/>
-      <c r="AF63" s="5"/>
-      <c r="AG63" s="5"/>
+      <c r="AE63" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="AF63" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="AG63" s="5" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="64" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
@@ -5952,8 +5955,6 @@
       <c r="P66" s="5"/>
       <c r="Q66" s="5"/>
       <c r="R66" s="5"/>
-      <c r="Z66" s="5"/>
-      <c r="AA66" s="5"/>
       <c r="AE66" s="5"/>
       <c r="AF66" s="5"/>
       <c r="AG66" s="5"/>
@@ -5977,7 +5978,8 @@
       <c r="P67" s="5"/>
       <c r="Q67" s="5"/>
       <c r="R67" s="5"/>
-      <c r="S67" s="5"/>
+      <c r="Z67" s="5"/>
+      <c r="AA67" s="5"/>
       <c r="AE67" s="5"/>
       <c r="AF67" s="5"/>
       <c r="AG67" s="5"/>
@@ -6001,6 +6003,7 @@
       <c r="P68" s="5"/>
       <c r="Q68" s="5"/>
       <c r="R68" s="5"/>
+      <c r="S68" s="5"/>
       <c r="AE68" s="5"/>
       <c r="AF68" s="5"/>
       <c r="AG68" s="5"/>
@@ -6033,8 +6036,14 @@
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
       <c r="G70" s="5"/>
       <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
       <c r="M70" s="5"/>
       <c r="N70" s="5"/>
       <c r="O70" s="5"/>
@@ -6049,7 +6058,7 @@
       <c r="A71" s="5"/>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
-      <c r="E71" s="5"/>
+      <c r="D71" s="5"/>
       <c r="G71" s="5"/>
       <c r="H71" s="5"/>
       <c r="M71" s="5"/>
@@ -6100,15 +6109,9 @@
       <c r="A74" s="5"/>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
       <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
       <c r="G74" s="5"/>
       <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
-      <c r="J74" s="5"/>
-      <c r="K74" s="5"/>
-      <c r="L74" s="5"/>
       <c r="M74" s="5"/>
       <c r="N74" s="5"/>
       <c r="O74" s="5"/>
@@ -6373,44 +6376,44 @@
       <c r="AG85" s="5"/>
     </row>
     <row r="86" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A86" s="6"/>
-      <c r="B86" s="6"/>
-      <c r="C86" s="6"/>
-      <c r="D86" s="6"/>
-      <c r="E86" s="6"/>
-      <c r="F86" s="6"/>
-      <c r="G86" s="6"/>
-      <c r="H86" s="6"/>
-      <c r="I86" s="6"/>
-      <c r="J86" s="6"/>
-      <c r="K86" s="6"/>
-      <c r="L86" s="6"/>
-      <c r="M86" s="6"/>
-      <c r="N86" s="6"/>
-      <c r="O86" s="6"/>
-      <c r="P86" s="7"/>
-      <c r="Q86" s="7"/>
-      <c r="R86" s="7"/>
+      <c r="A86" s="5"/>
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5"/>
+      <c r="H86" s="5"/>
+      <c r="I86" s="5"/>
+      <c r="J86" s="5"/>
+      <c r="K86" s="5"/>
+      <c r="L86" s="5"/>
+      <c r="M86" s="5"/>
+      <c r="N86" s="5"/>
+      <c r="O86" s="5"/>
+      <c r="P86" s="5"/>
+      <c r="Q86" s="5"/>
+      <c r="R86" s="5"/>
       <c r="AE86" s="5"/>
       <c r="AF86" s="5"/>
       <c r="AG86" s="5"/>
     </row>
     <row r="87" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A87" s="7"/>
-      <c r="B87" s="7"/>
-      <c r="C87" s="7"/>
-      <c r="D87" s="7"/>
-      <c r="E87" s="7"/>
-      <c r="F87" s="7"/>
-      <c r="G87" s="7"/>
-      <c r="H87" s="7"/>
-      <c r="I87" s="7"/>
-      <c r="J87" s="7"/>
-      <c r="K87" s="7"/>
-      <c r="L87" s="7"/>
-      <c r="M87" s="7"/>
-      <c r="N87" s="7"/>
-      <c r="O87" s="7"/>
+      <c r="A87" s="6"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="6"/>
+      <c r="K87" s="6"/>
+      <c r="L87" s="6"/>
+      <c r="M87" s="6"/>
+      <c r="N87" s="6"/>
+      <c r="O87" s="6"/>
       <c r="P87" s="7"/>
       <c r="Q87" s="7"/>
       <c r="R87" s="7"/>
@@ -6419,24 +6422,24 @@
       <c r="AG87" s="5"/>
     </row>
     <row r="88" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A88" s="5"/>
-      <c r="B88" s="5"/>
-      <c r="C88" s="5"/>
-      <c r="D88" s="5"/>
-      <c r="E88" s="5"/>
-      <c r="F88" s="5"/>
-      <c r="G88" s="5"/>
-      <c r="H88" s="5"/>
-      <c r="I88" s="5"/>
-      <c r="J88" s="5"/>
-      <c r="K88" s="5"/>
-      <c r="L88" s="5"/>
-      <c r="M88" s="5"/>
-      <c r="N88" s="5"/>
-      <c r="O88" s="5"/>
-      <c r="P88" s="5"/>
-      <c r="Q88" s="5"/>
-      <c r="R88" s="5"/>
+      <c r="A88" s="7"/>
+      <c r="B88" s="7"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="7"/>
+      <c r="E88" s="7"/>
+      <c r="F88" s="7"/>
+      <c r="G88" s="7"/>
+      <c r="H88" s="7"/>
+      <c r="I88" s="7"/>
+      <c r="J88" s="7"/>
+      <c r="K88" s="7"/>
+      <c r="L88" s="7"/>
+      <c r="M88" s="7"/>
+      <c r="N88" s="7"/>
+      <c r="O88" s="7"/>
+      <c r="P88" s="7"/>
+      <c r="Q88" s="7"/>
+      <c r="R88" s="7"/>
       <c r="AE88" s="5"/>
       <c r="AF88" s="5"/>
       <c r="AG88" s="5"/>
@@ -6534,90 +6537,90 @@
       <c r="AG92" s="5"/>
     </row>
     <row r="93" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A93" s="7"/>
-      <c r="B93" s="7"/>
-      <c r="C93" s="7"/>
-      <c r="D93" s="7"/>
-      <c r="E93" s="7"/>
-      <c r="F93" s="7"/>
-      <c r="G93" s="7"/>
-      <c r="H93" s="7"/>
-      <c r="I93" s="7"/>
-      <c r="J93" s="7"/>
-      <c r="K93" s="7"/>
-      <c r="L93" s="7"/>
-      <c r="M93" s="7"/>
-      <c r="N93" s="7"/>
-      <c r="O93" s="7"/>
-      <c r="P93" s="7"/>
-      <c r="Q93" s="7"/>
-      <c r="R93" s="7"/>
+      <c r="A93" s="5"/>
+      <c r="B93" s="5"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="5"/>
+      <c r="F93" s="5"/>
+      <c r="G93" s="5"/>
+      <c r="H93" s="5"/>
+      <c r="I93" s="5"/>
+      <c r="J93" s="5"/>
+      <c r="K93" s="5"/>
+      <c r="L93" s="5"/>
+      <c r="M93" s="5"/>
+      <c r="N93" s="5"/>
+      <c r="O93" s="5"/>
+      <c r="P93" s="5"/>
+      <c r="Q93" s="5"/>
+      <c r="R93" s="5"/>
       <c r="AE93" s="5"/>
       <c r="AF93" s="5"/>
       <c r="AG93" s="5"/>
     </row>
     <row r="94" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A94" s="5"/>
-      <c r="B94" s="5"/>
-      <c r="C94" s="5"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="5"/>
-      <c r="F94" s="5"/>
-      <c r="G94" s="5"/>
-      <c r="H94" s="5"/>
-      <c r="I94" s="5"/>
-      <c r="J94" s="5"/>
-      <c r="K94" s="5"/>
-      <c r="L94" s="5"/>
-      <c r="M94" s="5"/>
-      <c r="N94" s="5"/>
-      <c r="O94" s="5"/>
-      <c r="P94" s="5"/>
-      <c r="Q94" s="5"/>
-      <c r="R94" s="5"/>
+      <c r="A94" s="7"/>
+      <c r="B94" s="7"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="7"/>
+      <c r="F94" s="7"/>
+      <c r="G94" s="7"/>
+      <c r="H94" s="7"/>
+      <c r="I94" s="7"/>
+      <c r="J94" s="7"/>
+      <c r="K94" s="7"/>
+      <c r="L94" s="7"/>
+      <c r="M94" s="7"/>
+      <c r="N94" s="7"/>
+      <c r="O94" s="7"/>
+      <c r="P94" s="7"/>
+      <c r="Q94" s="7"/>
+      <c r="R94" s="7"/>
       <c r="AE94" s="5"/>
       <c r="AF94" s="5"/>
       <c r="AG94" s="5"/>
     </row>
     <row r="95" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A95" s="6"/>
-      <c r="B95" s="6"/>
-      <c r="C95" s="6"/>
-      <c r="D95" s="6"/>
-      <c r="E95" s="6"/>
-      <c r="F95" s="6"/>
-      <c r="G95" s="6"/>
-      <c r="H95" s="6"/>
-      <c r="I95" s="6"/>
-      <c r="J95" s="6"/>
-      <c r="K95" s="6"/>
-      <c r="L95" s="6"/>
-      <c r="M95" s="6"/>
-      <c r="N95" s="6"/>
-      <c r="O95" s="6"/>
-      <c r="P95" s="7"/>
-      <c r="Q95" s="7"/>
-      <c r="R95" s="7"/>
+      <c r="A95" s="5"/>
+      <c r="B95" s="5"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="5"/>
+      <c r="G95" s="5"/>
+      <c r="H95" s="5"/>
+      <c r="I95" s="5"/>
+      <c r="J95" s="5"/>
+      <c r="K95" s="5"/>
+      <c r="L95" s="5"/>
+      <c r="M95" s="5"/>
+      <c r="N95" s="5"/>
+      <c r="O95" s="5"/>
+      <c r="P95" s="5"/>
+      <c r="Q95" s="5"/>
+      <c r="R95" s="5"/>
       <c r="AE95" s="5"/>
       <c r="AF95" s="5"/>
       <c r="AG95" s="5"/>
     </row>
     <row r="96" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A96" s="7"/>
-      <c r="B96" s="7"/>
-      <c r="C96" s="7"/>
-      <c r="D96" s="7"/>
-      <c r="E96" s="7"/>
-      <c r="F96" s="7"/>
-      <c r="G96" s="7"/>
-      <c r="H96" s="7"/>
-      <c r="I96" s="7"/>
-      <c r="J96" s="7"/>
-      <c r="K96" s="7"/>
-      <c r="L96" s="7"/>
-      <c r="M96" s="7"/>
-      <c r="N96" s="7"/>
-      <c r="O96" s="7"/>
+      <c r="A96" s="6"/>
+      <c r="B96" s="6"/>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+      <c r="J96" s="6"/>
+      <c r="K96" s="6"/>
+      <c r="L96" s="6"/>
+      <c r="M96" s="6"/>
+      <c r="N96" s="6"/>
+      <c r="O96" s="6"/>
       <c r="P96" s="7"/>
       <c r="Q96" s="7"/>
       <c r="R96" s="7"/>
@@ -6626,24 +6629,24 @@
       <c r="AG96" s="5"/>
     </row>
     <row r="97" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A97" s="5"/>
-      <c r="B97" s="5"/>
-      <c r="C97" s="5"/>
-      <c r="D97" s="5"/>
-      <c r="E97" s="5"/>
-      <c r="F97" s="5"/>
-      <c r="G97" s="5"/>
-      <c r="H97" s="5"/>
-      <c r="I97" s="5"/>
-      <c r="J97" s="5"/>
-      <c r="K97" s="5"/>
-      <c r="L97" s="5"/>
-      <c r="M97" s="5"/>
-      <c r="N97" s="5"/>
-      <c r="O97" s="5"/>
-      <c r="P97" s="5"/>
-      <c r="Q97" s="5"/>
-      <c r="R97" s="5"/>
+      <c r="A97" s="7"/>
+      <c r="B97" s="7"/>
+      <c r="C97" s="7"/>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
+      <c r="F97" s="7"/>
+      <c r="G97" s="7"/>
+      <c r="H97" s="7"/>
+      <c r="I97" s="7"/>
+      <c r="J97" s="7"/>
+      <c r="K97" s="7"/>
+      <c r="L97" s="7"/>
+      <c r="M97" s="7"/>
+      <c r="N97" s="7"/>
+      <c r="O97" s="7"/>
+      <c r="P97" s="7"/>
+      <c r="Q97" s="7"/>
+      <c r="R97" s="7"/>
       <c r="AE97" s="5"/>
       <c r="AF97" s="5"/>
       <c r="AG97" s="5"/>
@@ -7201,47 +7204,47 @@
       <c r="AG121" s="5"/>
     </row>
     <row r="122" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A122" s="7"/>
-      <c r="B122" s="7"/>
-      <c r="C122" s="7"/>
-      <c r="D122" s="7"/>
-      <c r="E122" s="7"/>
-      <c r="F122" s="7"/>
-      <c r="G122" s="7"/>
-      <c r="H122" s="7"/>
-      <c r="I122" s="7"/>
-      <c r="J122" s="7"/>
-      <c r="K122" s="7"/>
-      <c r="L122" s="7"/>
-      <c r="M122" s="7"/>
-      <c r="N122" s="7"/>
-      <c r="O122" s="7"/>
-      <c r="P122" s="7"/>
-      <c r="Q122" s="7"/>
-      <c r="R122" s="7"/>
+      <c r="A122" s="5"/>
+      <c r="B122" s="5"/>
+      <c r="C122" s="5"/>
+      <c r="D122" s="5"/>
+      <c r="E122" s="5"/>
+      <c r="F122" s="5"/>
+      <c r="G122" s="5"/>
+      <c r="H122" s="5"/>
+      <c r="I122" s="5"/>
+      <c r="J122" s="5"/>
+      <c r="K122" s="5"/>
+      <c r="L122" s="5"/>
+      <c r="M122" s="5"/>
+      <c r="N122" s="5"/>
+      <c r="O122" s="5"/>
+      <c r="P122" s="5"/>
+      <c r="Q122" s="5"/>
+      <c r="R122" s="5"/>
       <c r="AE122" s="5"/>
       <c r="AF122" s="5"/>
       <c r="AG122" s="5"/>
     </row>
     <row r="123" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A123" s="5"/>
-      <c r="B123" s="5"/>
-      <c r="C123" s="5"/>
-      <c r="D123" s="5"/>
-      <c r="E123" s="5"/>
-      <c r="F123" s="5"/>
-      <c r="G123" s="5"/>
-      <c r="H123" s="5"/>
-      <c r="I123" s="5"/>
-      <c r="J123" s="5"/>
-      <c r="K123" s="5"/>
-      <c r="L123" s="5"/>
-      <c r="M123" s="5"/>
-      <c r="N123" s="5"/>
-      <c r="O123" s="5"/>
-      <c r="P123" s="5"/>
-      <c r="Q123" s="5"/>
-      <c r="R123" s="5"/>
+      <c r="A123" s="7"/>
+      <c r="B123" s="7"/>
+      <c r="C123" s="7"/>
+      <c r="D123" s="7"/>
+      <c r="E123" s="7"/>
+      <c r="F123" s="7"/>
+      <c r="G123" s="7"/>
+      <c r="H123" s="7"/>
+      <c r="I123" s="7"/>
+      <c r="J123" s="7"/>
+      <c r="K123" s="7"/>
+      <c r="L123" s="7"/>
+      <c r="M123" s="7"/>
+      <c r="N123" s="7"/>
+      <c r="O123" s="7"/>
+      <c r="P123" s="7"/>
+      <c r="Q123" s="7"/>
+      <c r="R123" s="7"/>
       <c r="AE123" s="5"/>
       <c r="AF123" s="5"/>
       <c r="AG123" s="5"/>
@@ -7684,47 +7687,47 @@
       <c r="AG142" s="5"/>
     </row>
     <row r="143" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A143" s="7"/>
-      <c r="B143" s="7"/>
-      <c r="C143" s="7"/>
-      <c r="D143" s="7"/>
-      <c r="E143" s="7"/>
-      <c r="F143" s="7"/>
-      <c r="G143" s="7"/>
-      <c r="H143" s="7"/>
-      <c r="I143" s="7"/>
-      <c r="J143" s="7"/>
-      <c r="K143" s="7"/>
-      <c r="L143" s="7"/>
-      <c r="M143" s="7"/>
-      <c r="N143" s="7"/>
-      <c r="O143" s="7"/>
-      <c r="P143" s="7"/>
-      <c r="Q143" s="7"/>
-      <c r="R143" s="7"/>
+      <c r="A143" s="5"/>
+      <c r="B143" s="5"/>
+      <c r="C143" s="5"/>
+      <c r="D143" s="5"/>
+      <c r="E143" s="5"/>
+      <c r="F143" s="5"/>
+      <c r="G143" s="5"/>
+      <c r="H143" s="5"/>
+      <c r="I143" s="5"/>
+      <c r="J143" s="5"/>
+      <c r="K143" s="5"/>
+      <c r="L143" s="5"/>
+      <c r="M143" s="5"/>
+      <c r="N143" s="5"/>
+      <c r="O143" s="5"/>
+      <c r="P143" s="5"/>
+      <c r="Q143" s="5"/>
+      <c r="R143" s="5"/>
       <c r="AE143" s="5"/>
       <c r="AF143" s="5"/>
       <c r="AG143" s="5"/>
     </row>
     <row r="144" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A144" s="5"/>
-      <c r="B144" s="5"/>
-      <c r="C144" s="5"/>
-      <c r="D144" s="5"/>
-      <c r="E144" s="5"/>
-      <c r="F144" s="5"/>
-      <c r="G144" s="5"/>
-      <c r="H144" s="5"/>
-      <c r="I144" s="5"/>
-      <c r="J144" s="5"/>
-      <c r="K144" s="5"/>
-      <c r="L144" s="5"/>
-      <c r="M144" s="5"/>
-      <c r="N144" s="5"/>
-      <c r="O144" s="5"/>
-      <c r="P144" s="5"/>
-      <c r="Q144" s="5"/>
-      <c r="R144" s="5"/>
+      <c r="A144" s="7"/>
+      <c r="B144" s="7"/>
+      <c r="C144" s="7"/>
+      <c r="D144" s="7"/>
+      <c r="E144" s="7"/>
+      <c r="F144" s="7"/>
+      <c r="G144" s="7"/>
+      <c r="H144" s="7"/>
+      <c r="I144" s="7"/>
+      <c r="J144" s="7"/>
+      <c r="K144" s="7"/>
+      <c r="L144" s="7"/>
+      <c r="M144" s="7"/>
+      <c r="N144" s="7"/>
+      <c r="O144" s="7"/>
+      <c r="P144" s="7"/>
+      <c r="Q144" s="7"/>
+      <c r="R144" s="7"/>
       <c r="AE144" s="5"/>
       <c r="AF144" s="5"/>
       <c r="AG144" s="5"/>
@@ -8211,9 +8214,32 @@
       <c r="AE165" s="5"/>
       <c r="AF165" s="5"/>
       <c r="AG165" s="5"/>
-      <c r="AH165" s="5"/>
-      <c r="AI165" s="5"/>
-      <c r="AJ165" s="5"/>
+    </row>
+    <row r="166" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A166" s="5"/>
+      <c r="B166" s="5"/>
+      <c r="C166" s="5"/>
+      <c r="D166" s="5"/>
+      <c r="E166" s="5"/>
+      <c r="F166" s="5"/>
+      <c r="G166" s="5"/>
+      <c r="H166" s="5"/>
+      <c r="I166" s="5"/>
+      <c r="J166" s="5"/>
+      <c r="K166" s="5"/>
+      <c r="L166" s="5"/>
+      <c r="M166" s="5"/>
+      <c r="N166" s="5"/>
+      <c r="O166" s="5"/>
+      <c r="P166" s="5"/>
+      <c r="Q166" s="5"/>
+      <c r="R166" s="5"/>
+      <c r="AE166" s="5"/>
+      <c r="AF166" s="5"/>
+      <c r="AG166" s="5"/>
+      <c r="AH166" s="5"/>
+      <c r="AI166" s="5"/>
+      <c r="AJ166" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8228,7 +8254,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961E221B-EB6D-4BE8-BFFD-B04ECD18E636}">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -8255,7 +8281,7 @@
     </row>
     <row r="2" spans="1:5" ht="219" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="91" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="B2" s="91"/>
       <c r="C2" s="91"/>
@@ -8264,7 +8290,7 @@
     </row>
     <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="92" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B3" s="92"/>
       <c r="C3" s="92"/>
@@ -8273,7 +8299,7 @@
     </row>
     <row r="4" spans="1:5" ht="371.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="91" t="s">
-        <v>240</v>
+        <v>279</v>
       </c>
       <c r="B4" s="91"/>
       <c r="C4" s="91"/>
@@ -8306,7 +8332,7 @@
       </c>
       <c r="C6" s="33"/>
       <c r="D6" s="34" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E6" s="35" t="s">
         <v>161</v>
@@ -8319,7 +8345,7 @@
       </c>
       <c r="C7" s="36"/>
       <c r="D7" s="37" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="E7" s="38" t="s">
         <v>175</v>
@@ -8357,14 +8383,14 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="B10" s="33" t="s">
         <v>174</v>
       </c>
       <c r="C10" s="33"/>
       <c r="D10" s="34" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="E10" s="35" t="s">
         <v>175</v>
@@ -8405,7 +8431,7 @@
       </c>
       <c r="C13" s="33"/>
       <c r="D13" s="34" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="E13" s="38" t="s">
         <v>175</v>
@@ -8545,11 +8571,11 @@
     <row r="23" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="44"/>
       <c r="B23" s="44" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="C23" s="44"/>
       <c r="D23" s="45" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="E23" s="46" t="s">
         <v>175</v>
@@ -8601,10 +8627,10 @@
         <v>200</v>
       </c>
       <c r="D27" s="59" t="s">
+        <v>201</v>
+      </c>
+      <c r="E27" s="35" t="s">
         <v>202</v>
-      </c>
-      <c r="E27" s="35" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
@@ -8638,7 +8664,7 @@
       <c r="D30" s="88"/>
       <c r="E30" s="89"/>
     </row>
-    <row r="31" spans="1:5" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="229.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="54" t="s">
         <v>123</v>
       </c>
@@ -8646,7 +8672,7 @@
         <v>145</v>
       </c>
       <c r="C31" s="75" t="s">
-        <v>235</v>
+        <v>289</v>
       </c>
       <c r="D31" s="76"/>
       <c r="E31" s="77"/>
@@ -8659,7 +8685,7 @@
         <v>146</v>
       </c>
       <c r="C32" s="78" t="s">
-        <v>234</v>
+        <v>281</v>
       </c>
       <c r="D32" s="79"/>
       <c r="E32" s="80"/>
@@ -8672,7 +8698,7 @@
         <v>147</v>
       </c>
       <c r="C33" s="81" t="s">
-        <v>233</v>
+        <v>284</v>
       </c>
       <c r="D33" s="82"/>
       <c r="E33" s="83"/>
@@ -8711,7 +8737,7 @@
         <v>150</v>
       </c>
       <c r="C36" s="72" t="s">
-        <v>232</v>
+        <v>287</v>
       </c>
       <c r="D36" s="73"/>
       <c r="E36" s="74"/>
@@ -8737,7 +8763,7 @@
         <v>152</v>
       </c>
       <c r="C38" s="66" t="s">
-        <v>231</v>
+        <v>288</v>
       </c>
       <c r="D38" s="67"/>
       <c r="E38" s="68"/>
@@ -8780,21 +8806,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>273</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>163</v>
+        <v>274</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
         <v>198</v>
       </c>
     </row>
@@ -8827,10 +8848,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B976463-CB67-4980-A3BF-97B6150247F7}">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8854,7 +8875,7 @@
     </row>
     <row r="2" spans="1:5" ht="216" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="91" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="B2" s="91"/>
       <c r="C2" s="91"/>
@@ -8863,7 +8884,7 @@
     </row>
     <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="92" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B3" s="92"/>
       <c r="C3" s="92"/>
@@ -8872,7 +8893,7 @@
     </row>
     <row r="4" spans="1:5" ht="380.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="91" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
       <c r="B4" s="91"/>
       <c r="C4" s="91"/>
@@ -8881,19 +8902,19 @@
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="51" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" s="52" t="s">
         <v>210</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="C5" s="52" t="s">
         <v>211</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="D5" s="52" t="s">
         <v>212</v>
       </c>
-      <c r="D5" s="52" t="s">
-        <v>213</v>
-      </c>
       <c r="E5" s="53" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -8905,10 +8926,10 @@
       </c>
       <c r="C6" s="33"/>
       <c r="D6" s="34" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -8918,7 +8939,7 @@
       </c>
       <c r="C7" s="36"/>
       <c r="D7" s="37" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="E7" s="38" t="s">
         <v>175</v>
@@ -8933,10 +8954,10 @@
       </c>
       <c r="C8" s="33"/>
       <c r="D8" s="34" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -8948,22 +8969,22 @@
       </c>
       <c r="C9" s="33"/>
       <c r="D9" s="34" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="B10" s="33" t="s">
         <v>174</v>
       </c>
       <c r="C10" s="33"/>
       <c r="D10" s="34" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="E10" s="35" t="s">
         <v>175</v>
@@ -8978,10 +8999,10 @@
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="34" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -8991,7 +9012,7 @@
       </c>
       <c r="C12" s="33"/>
       <c r="D12" s="34" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E12" s="35" t="s">
         <v>175</v>
@@ -9004,7 +9025,7 @@
       </c>
       <c r="C13" s="33"/>
       <c r="D13" s="34" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="E13" s="38" t="s">
         <v>175</v>
@@ -9019,10 +9040,10 @@
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="40" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E14" s="41" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -9032,7 +9053,7 @@
       </c>
       <c r="C15" s="42"/>
       <c r="D15" s="43" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="E15" s="38" t="s">
         <v>175</v>
@@ -9047,10 +9068,10 @@
       </c>
       <c r="C16" s="33"/>
       <c r="D16" s="34" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -9062,10 +9083,10 @@
       </c>
       <c r="C17" s="36"/>
       <c r="D17" s="37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -9077,10 +9098,10 @@
       </c>
       <c r="C18" s="33"/>
       <c r="D18" s="34" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E18" s="35" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -9092,10 +9113,10 @@
       </c>
       <c r="C19" s="33"/>
       <c r="D19" s="34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -9105,7 +9126,7 @@
       </c>
       <c r="C20" s="36"/>
       <c r="D20" s="37" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="E20" s="38" t="s">
         <v>175</v>
@@ -9120,10 +9141,10 @@
       </c>
       <c r="C21" s="33"/>
       <c r="D21" s="34" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E21" s="35" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -9135,20 +9156,20 @@
       </c>
       <c r="C22" s="36"/>
       <c r="D22" s="37" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="E22" s="38" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="44"/>
       <c r="B23" s="44" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="C23" s="44"/>
       <c r="D23" s="45" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="E23" s="46" t="s">
         <v>175</v>
@@ -9161,10 +9182,10 @@
         <v>19</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="E24" s="47" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -9174,10 +9195,10 @@
         <v>47</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="E25" s="47" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -9187,10 +9208,10 @@
         <v>35</v>
       </c>
       <c r="D26" s="49" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="E26" s="47" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="120" x14ac:dyDescent="0.25">
@@ -9200,15 +9221,15 @@
         <v>200</v>
       </c>
       <c r="D27" s="50" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="E27" s="38" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -9217,7 +9238,7 @@
     </row>
     <row r="29" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="91" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="B29" s="91"/>
       <c r="C29" s="91"/>
@@ -9226,26 +9247,26 @@
     </row>
     <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="31" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B30" s="32" t="s">
         <v>124</v>
       </c>
       <c r="C30" s="87" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D30" s="88"/>
       <c r="E30" s="89"/>
     </row>
-    <row r="31" spans="1:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="217.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="54" t="s">
         <v>123</v>
       </c>
       <c r="B31" s="54" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C31" s="75" t="s">
-        <v>266</v>
+        <v>280</v>
       </c>
       <c r="D31" s="76"/>
       <c r="E31" s="77"/>
@@ -9255,10 +9276,10 @@
         <v>175</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C32" s="78" t="s">
-        <v>267</v>
+        <v>282</v>
       </c>
       <c r="D32" s="79"/>
       <c r="E32" s="80"/>
@@ -9268,10 +9289,10 @@
         <v>125</v>
       </c>
       <c r="B33" s="55" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C33" s="81" t="s">
-        <v>255</v>
+        <v>283</v>
       </c>
       <c r="D33" s="82"/>
       <c r="E33" s="83"/>
@@ -9281,10 +9302,10 @@
         <v>126</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C34" s="84" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="D34" s="85"/>
       <c r="E34" s="86"/>
@@ -9294,10 +9315,10 @@
         <v>127</v>
       </c>
       <c r="B35" s="57" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C35" s="69" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="D35" s="70"/>
       <c r="E35" s="71"/>
@@ -9307,10 +9328,10 @@
         <v>128</v>
       </c>
       <c r="B36" s="29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C36" s="72" t="s">
-        <v>257</v>
+        <v>285</v>
       </c>
       <c r="D36" s="73"/>
       <c r="E36" s="74"/>
@@ -9320,10 +9341,10 @@
         <v>178</v>
       </c>
       <c r="B37" s="58" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="C37" s="63" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="D37" s="64"/>
       <c r="E37" s="65"/>
@@ -9333,10 +9354,10 @@
         <v>179</v>
       </c>
       <c r="B38" s="29" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="C38" s="66" t="s">
-        <v>259</v>
+        <v>286</v>
       </c>
       <c r="D38" s="67"/>
       <c r="E38" s="68"/>
@@ -9346,10 +9367,10 @@
         <v>180</v>
       </c>
       <c r="B39" s="56" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="C39" s="69" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="D39" s="70"/>
       <c r="E39" s="71"/>
@@ -9359,42 +9380,37 @@
         <v>181</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="C40" s="72" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="D40" s="73"/>
       <c r="E40" s="74"/>
     </row>
     <row r="41" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>260</v>
+        <v>273</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: enable name definition per specification
Inclusion of a new column "SpecificationName" to define IFC versions row wise.
</commit_message>
<xml_diff>
--- a/Excel-files/IDS4ALL-Template.xlsx
+++ b/Excel-files/IDS4ALL-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5cb7fc635d7635b3/Dokumente/01-Eigene-Dateien/TU-Wien/05-Projekte/2022-AIA4All/IDS/IDS-converter/Excel-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="470" documentId="13_ncr:1_{1B5B4233-0C82-414A-875B-768DAFFA80D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{566386A2-FD66-4F3A-AD01-3C6800015D75}"/>
+  <xr:revisionPtr revIDLastSave="519" documentId="13_ncr:1_{1B5B4233-0C82-414A-875B-768DAFFA80D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E5A5EF4-BBC3-4503-B44A-B0866E4D90E4}"/>
   <bookViews>
-    <workbookView xWindow="-22597" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="4" xr2:uid="{16497593-A6A8-4643-B0B9-95B48379E78A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{16497593-A6A8-4643-B0B9-95B48379E78A}"/>
   </bookViews>
   <sheets>
     <sheet name="IDS4ALL" sheetId="20" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="298">
   <si>
     <t>IfcLabel</t>
   </si>
@@ -1074,12 +1074,6 @@
     <t>IfcWall.SOLIDWALL</t>
   </si>
   <si>
-    <t>Der Name einer Spezifikation kann nicht benutzerdefiniert festgelegt werden. Er wird aus der IFC-Entität automatisch erzeugt.</t>
-  </si>
-  <si>
-    <t>The name of a specification cannot be defined by the user. It is generated automatically from the IFC entity.</t>
-  </si>
-  <si>
     <t>IFC4,IFC4X3_ADD2</t>
   </si>
   <si>
@@ -1206,6 +1200,34 @@
   </si>
   <si>
     <t>Defining custom values for the purpose and milestone of the IDS is not possible. These values are automatically generated from the general columns. The phases are saved as milestones and the combination of roles and use cases as purpose.</t>
+  </si>
+  <si>
+    <t>SpecificationName</t>
+  </si>
+  <si>
+    <t>Attika</t>
+  </si>
+  <si>
+    <t>Wall-general</t>
+  </si>
+  <si>
+    <t>Wall-non-bearing</t>
+  </si>
+  <si>
+    <t>Wall-load-bearing</t>
+  </si>
+  <si>
+    <t>Definition des Spezifikationsnamen. Spezifikationen mit unterschiedlichen Namen werden nicht zusammengefügt, auch wenn die Applicability und die anderen allgemeinen Daten gleich sind.
+Eine Ausnahme besteht für die Zusammenführung von spezifischeren zu allgemeinen Werten. Hier wid der Name der allgemeineren Spezifikation durch den Namen der spezifischeren ersetzt. In den "Example sepcifications" werden trotz unterschiedlicher Namen die Zeilen 10 und 11 mit 12-21 sowie mit 22-31 zusammengeführt und die spezifischeren Namen verwendet.
+Spezifikationen ohne definierten Namen werden durchnummeriert und mit der Entität ergänzt.</t>
+  </si>
+  <si>
+    <t>Definition of the specification name. Specifications with different names are not merged, even if the applicability and other general data are the same.
+An exception is made for merging more specific values with more general ones. In this case, the name of the more general specification is replaced by the name of the more specific one. In the ‘Example specifications’, despite having different names, lines 10 and 11 are merged with 12-21 and 22-31, and the more specific names are used.
+Specifications without a defined name are numbered consecutively and supplemented with the entity.</t>
+  </si>
+  <si>
+    <t>External-wall-awmhhi01a-03</t>
   </si>
 </sst>
 </file>
@@ -1636,7 +1658,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1798,6 +1820,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2195,13 +2220,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{1ACD0757-A577-40EE-9289-2CCF213FB5DB}" name="Tabelle8" displayName="Tabelle8" ref="A5:E28" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13">
-  <autoFilter ref="A5:E28" xr:uid="{1ACD0757-A577-40EE-9289-2CCF213FB5DB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{1ACD0757-A577-40EE-9289-2CCF213FB5DB}" name="Tabelle8" displayName="Tabelle8" ref="A5:E29" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13">
+  <autoFilter ref="A5:E29" xr:uid="{1ACD0757-A577-40EE-9289-2CCF213FB5DB}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B9152E4C-9FDE-4F2B-B749-435F41490348}" name="Applicability column names " dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{AC490DC2-16A5-4694-A843-59073F28FA54}" name="Requirements column names" dataDxfId="11"/>
@@ -2214,8 +2235,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2B550DFF-9D6B-4283-B858-1FF97DFDC130}" name="Tabelle2" displayName="Tabelle2" ref="A5:E28" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
-  <autoFilter ref="A5:E28" xr:uid="{2B550DFF-9D6B-4283-B858-1FF97DFDC130}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2B550DFF-9D6B-4283-B858-1FF97DFDC130}" name="Tabelle2" displayName="Tabelle2" ref="A5:E29" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
+  <autoFilter ref="A5:E29" xr:uid="{2B550DFF-9D6B-4283-B858-1FF97DFDC130}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{4B793972-3BEC-40A4-95D5-FD10FE2CEC36}" name="Spaltennamen Applicability" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0C2D1FE8-BFBB-4D2A-AC83-881A04FD4E10}" name="Spaltennamen Requirements" dataDxfId="2"/>
@@ -2527,7 +2548,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2662,7 +2683,7 @@
         <v>79</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>71</v>
@@ -2671,7 +2692,7 @@
         <v>113</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2701,7 +2722,7 @@
         <v>261</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2722,7 +2743,7 @@
   <dimension ref="A1:AJ11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2762,41 +2783,42 @@
     <col min="33" max="33" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="65" t="s">
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="65"/>
-      <c r="AA1" s="65"/>
-      <c r="AB1" s="65"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
+      <c r="X1" s="66"/>
+      <c r="Y1" s="66"/>
+      <c r="Z1" s="66"/>
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="66"/>
       <c r="AC1" s="24"/>
       <c r="AD1" s="24"/>
       <c r="AE1" s="2"/>
@@ -2804,6 +2826,7 @@
       <c r="AG1" s="2"/>
       <c r="AH1" s="2"/>
       <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2909,7 +2932,10 @@
         <v>194</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
@@ -3136,8 +3162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134D532F-CD5A-45F4-AF33-42136DA547E7}">
   <dimension ref="A1:AJ166"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA31" sqref="AA31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3172,45 +3198,46 @@
     <col min="28" max="28" width="11.140625" customWidth="1"/>
     <col min="29" max="30" width="19" customWidth="1"/>
     <col min="31" max="31" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="65" t="s">
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="65"/>
-      <c r="AA1" s="65"/>
-      <c r="AB1" s="65"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
+      <c r="X1" s="66"/>
+      <c r="Y1" s="66"/>
+      <c r="Z1" s="66"/>
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="66"/>
       <c r="AC1" s="24"/>
       <c r="AD1" s="24"/>
       <c r="AE1" s="2"/>
@@ -3218,6 +3245,7 @@
       <c r="AG1" s="2"/>
       <c r="AH1" s="2"/>
       <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -3323,7 +3351,10 @@
         <v>194</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
@@ -3444,7 +3475,7 @@
         <v>71</v>
       </c>
       <c r="AI5" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:36" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3481,7 +3512,7 @@
         <v>71</v>
       </c>
       <c r="AI6" s="12" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
@@ -3526,7 +3557,7 @@
         <v>71</v>
       </c>
       <c r="AI7" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="AJ7" s="5"/>
     </row>
@@ -3570,7 +3601,7 @@
         <v>71</v>
       </c>
       <c r="AI8" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="AJ8" s="5"/>
     </row>
@@ -3663,7 +3694,9 @@
       </c>
       <c r="AH10" s="5"/>
       <c r="AI10" s="5"/>
-      <c r="AJ10" s="5"/>
+      <c r="AJ10" s="5" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -3713,7 +3746,9 @@
       </c>
       <c r="AH11" s="5"/>
       <c r="AI11" s="5"/>
-      <c r="AJ11" s="5"/>
+      <c r="AJ11" s="5" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -3761,7 +3796,9 @@
         <v>166</v>
       </c>
       <c r="AI12" s="5"/>
-      <c r="AJ12" s="5"/>
+      <c r="AJ12" s="5" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -3810,7 +3847,9 @@
         <v>166</v>
       </c>
       <c r="AI13" s="5"/>
-      <c r="AJ13" s="5"/>
+      <c r="AJ13" s="5" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -3859,7 +3898,9 @@
         <v>166</v>
       </c>
       <c r="AI14" s="5"/>
-      <c r="AJ14" s="5"/>
+      <c r="AJ14" s="5" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -3908,7 +3949,9 @@
         <v>166</v>
       </c>
       <c r="AI15" s="5"/>
-      <c r="AJ15" s="5"/>
+      <c r="AJ15" s="5" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -3957,7 +4000,9 @@
         <v>166</v>
       </c>
       <c r="AI16" s="5"/>
-      <c r="AJ16" s="5"/>
+      <c r="AJ16" s="5" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
@@ -4006,7 +4051,9 @@
         <v>166</v>
       </c>
       <c r="AI17" s="5"/>
-      <c r="AJ17" s="5"/>
+      <c r="AJ17" s="5" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
@@ -4055,7 +4102,9 @@
         <v>166</v>
       </c>
       <c r="AI18" s="5"/>
-      <c r="AJ18" s="5"/>
+      <c r="AJ18" s="5" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
@@ -4104,7 +4153,9 @@
         <v>166</v>
       </c>
       <c r="AI19" s="5"/>
-      <c r="AJ19" s="5"/>
+      <c r="AJ19" s="5" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -4154,7 +4205,9 @@
       </c>
       <c r="AH20" s="5"/>
       <c r="AI20" s="5"/>
-      <c r="AJ20" s="5"/>
+      <c r="AJ20" s="5" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
@@ -4203,7 +4256,9 @@
         <v>166</v>
       </c>
       <c r="AI21" s="5"/>
-      <c r="AJ21" s="5"/>
+      <c r="AJ21" s="5" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -4252,7 +4307,9 @@
         <v>166</v>
       </c>
       <c r="AI22" s="5"/>
-      <c r="AJ22" s="5"/>
+      <c r="AJ22" s="5" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -4301,7 +4358,9 @@
         <v>166</v>
       </c>
       <c r="AI23" s="5"/>
-      <c r="AJ23" s="5"/>
+      <c r="AJ23" s="5" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
@@ -4352,7 +4411,9 @@
       </c>
       <c r="AH24" s="5"/>
       <c r="AI24" s="5"/>
-      <c r="AJ24" s="5"/>
+      <c r="AJ24" s="5" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -4401,7 +4462,9 @@
         <v>166</v>
       </c>
       <c r="AI25" s="5"/>
-      <c r="AJ25" s="5"/>
+      <c r="AJ25" s="5" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
@@ -4450,7 +4513,9 @@
         <v>166</v>
       </c>
       <c r="AI26" s="5"/>
-      <c r="AJ26" s="5"/>
+      <c r="AJ26" s="5" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
@@ -4499,7 +4564,9 @@
         <v>166</v>
       </c>
       <c r="AI27" s="5"/>
-      <c r="AJ27" s="5"/>
+      <c r="AJ27" s="5" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
@@ -4548,7 +4615,9 @@
         <v>166</v>
       </c>
       <c r="AI28" s="5"/>
-      <c r="AJ28" s="5"/>
+      <c r="AJ28" s="5" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
@@ -4597,7 +4666,9 @@
         <v>166</v>
       </c>
       <c r="AI29" s="5"/>
-      <c r="AJ29" s="5"/>
+      <c r="AJ29" s="5" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
@@ -4646,7 +4717,9 @@
         <v>166</v>
       </c>
       <c r="AI30" s="5"/>
-      <c r="AJ30" s="5"/>
+      <c r="AJ30" s="5" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
@@ -4695,7 +4768,9 @@
         <v>166</v>
       </c>
       <c r="AI31" s="5"/>
-      <c r="AJ31" s="5"/>
+      <c r="AJ31" s="5" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
@@ -4773,7 +4848,7 @@
     </row>
     <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -4781,10 +4856,10 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
@@ -4812,7 +4887,9 @@
         <v>166</v>
       </c>
       <c r="AI34" s="5"/>
-      <c r="AJ34" s="5"/>
+      <c r="AJ34" s="5" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
@@ -5052,7 +5129,7 @@
     </row>
     <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -5357,7 +5434,7 @@
       </c>
       <c r="AI48" s="5"/>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>86</v>
       </c>
@@ -5403,7 +5480,7 @@
       </c>
       <c r="AI49" s="5"/>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>86</v>
       </c>
@@ -5443,7 +5520,7 @@
       </c>
       <c r="AI50" s="5"/>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>86</v>
       </c>
@@ -5483,7 +5560,7 @@
       </c>
       <c r="AI51" s="5"/>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>86</v>
       </c>
@@ -5521,7 +5598,7 @@
       </c>
       <c r="AI52" s="5"/>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>86</v>
       </c>
@@ -5559,7 +5636,7 @@
       </c>
       <c r="AI53" s="5"/>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>86</v>
       </c>
@@ -5597,7 +5674,7 @@
       </c>
       <c r="AI54" s="5"/>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -5621,7 +5698,7 @@
       <c r="AG55" s="5"/>
       <c r="AI55" s="5"/>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>2</v>
       </c>
@@ -5664,8 +5741,11 @@
         <v>166</v>
       </c>
       <c r="AI56" s="5"/>
-    </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ56" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>2</v>
       </c>
@@ -5708,8 +5788,11 @@
         <v>166</v>
       </c>
       <c r="AI57" s="5"/>
-    </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ57" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>2</v>
       </c>
@@ -5752,8 +5835,11 @@
         <v>166</v>
       </c>
       <c r="AI58" s="5"/>
-    </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ58" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>2</v>
       </c>
@@ -5796,8 +5882,11 @@
         <v>166</v>
       </c>
       <c r="AI59" s="5"/>
-    </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ59" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>2</v>
       </c>
@@ -5840,8 +5929,11 @@
         <v>166</v>
       </c>
       <c r="AI60" s="5"/>
-    </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ60" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -5865,7 +5957,7 @@
       <c r="AG61" s="5"/>
       <c r="AI61" s="5"/>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>2</v>
       </c>
@@ -5909,7 +6001,7 @@
       </c>
       <c r="AI62" s="5"/>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>2</v>
       </c>
@@ -5953,7 +6045,7 @@
       </c>
       <c r="AI63" s="5"/>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
@@ -8421,7 +8513,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8435,39 +8527,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="94" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
       <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:5" ht="219" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="95" t="s">
         <v>249</v>
       </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
       <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="96" t="s">
         <v>196</v>
       </c>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
       <c r="E3" s="15"/>
     </row>
     <row r="4" spans="1:5" ht="371.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="94" t="s">
-        <v>288</v>
-      </c>
-      <c r="B4" s="94"/>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
+      <c r="A4" s="95" t="s">
+        <v>286</v>
+      </c>
+      <c r="B4" s="95"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
       <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8496,7 +8588,7 @@
       </c>
       <c r="C6" s="33"/>
       <c r="D6" s="34" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E6" s="35" t="s">
         <v>157</v>
@@ -8791,7 +8883,7 @@
         <v>194</v>
       </c>
       <c r="D27" s="59" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E27" s="35" t="s">
         <v>195</v>
@@ -8801,214 +8893,222 @@
       <c r="A28" s="33"/>
       <c r="B28" s="33"/>
       <c r="C28" s="39" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D28" s="62" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E28" s="35" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
+    <row r="29" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A29" s="33"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33" t="s">
+        <v>290</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>296</v>
+      </c>
+      <c r="E29" s="35" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-    </row>
-    <row r="30" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="94" t="s">
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+    </row>
+    <row r="31" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="95" t="s">
         <v>172</v>
       </c>
-      <c r="B30" s="94"/>
-      <c r="C30" s="94"/>
-      <c r="D30" s="94"/>
-      <c r="E30" s="94"/>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="31" t="s">
+      <c r="B31" s="95"/>
+      <c r="C31" s="95"/>
+      <c r="D31" s="95"/>
+      <c r="E31" s="95"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="B31" s="32" t="s">
+      <c r="B32" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="C31" s="90" t="s">
+      <c r="C32" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="D31" s="91"/>
-      <c r="E31" s="92"/>
-    </row>
-    <row r="32" spans="1:5" ht="229.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="54" t="s">
+      <c r="D32" s="92"/>
+      <c r="E32" s="93"/>
+    </row>
+    <row r="33" spans="1:5" ht="229.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="54" t="s">
         <v>119</v>
       </c>
-      <c r="B32" s="54" t="s">
+      <c r="B33" s="54" t="s">
         <v>141</v>
       </c>
-      <c r="C32" s="78" t="s">
-        <v>290</v>
-      </c>
-      <c r="D32" s="79"/>
-      <c r="E32" s="80"/>
-    </row>
-    <row r="33" spans="1:5" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="26" t="s">
+      <c r="C33" s="79" t="s">
+        <v>288</v>
+      </c>
+      <c r="D33" s="80"/>
+      <c r="E33" s="81"/>
+    </row>
+    <row r="34" spans="1:5" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B34" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="C33" s="81" t="s">
-        <v>270</v>
-      </c>
-      <c r="D33" s="82"/>
-      <c r="E33" s="83"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="55" t="s">
+      <c r="C34" s="82" t="s">
+        <v>268</v>
+      </c>
+      <c r="D34" s="83"/>
+      <c r="E34" s="84"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="B34" s="55" t="s">
+      <c r="B35" s="55" t="s">
         <v>143</v>
       </c>
-      <c r="C34" s="84" t="s">
-        <v>273</v>
-      </c>
-      <c r="D34" s="85"/>
-      <c r="E34" s="86"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="27" t="s">
+      <c r="C35" s="85" t="s">
+        <v>271</v>
+      </c>
+      <c r="D35" s="86"/>
+      <c r="E35" s="87"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B36" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="C35" s="87" t="s">
+      <c r="C36" s="88" t="s">
         <v>151</v>
       </c>
-      <c r="D35" s="88"/>
-      <c r="E35" s="89"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="56" t="s">
+      <c r="D36" s="89"/>
+      <c r="E36" s="90"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="56" t="s">
         <v>123</v>
       </c>
-      <c r="B36" s="56" t="s">
+      <c r="B37" s="56" t="s">
         <v>145</v>
       </c>
-      <c r="C36" s="72" t="s">
+      <c r="C37" s="73" t="s">
         <v>151</v>
       </c>
-      <c r="D36" s="73"/>
-      <c r="E36" s="74"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="28" t="s">
+      <c r="D37" s="74"/>
+      <c r="E37" s="75"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="B37" s="28" t="s">
+      <c r="B38" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="C37" s="75" t="s">
-        <v>276</v>
-      </c>
-      <c r="D37" s="76"/>
-      <c r="E37" s="77"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="58" t="s">
+      <c r="C38" s="76" t="s">
+        <v>274</v>
+      </c>
+      <c r="D38" s="77"/>
+      <c r="E38" s="78"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="58" t="s">
         <v>173</v>
       </c>
-      <c r="B38" s="58" t="s">
+      <c r="B39" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="C38" s="66" t="s">
+      <c r="C39" s="67" t="s">
         <v>152</v>
       </c>
-      <c r="D38" s="67"/>
-      <c r="E38" s="68"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="29" t="s">
+      <c r="D39" s="68"/>
+      <c r="E39" s="69"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="B39" s="29" t="s">
+      <c r="B40" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="C39" s="69" t="s">
-        <v>277</v>
-      </c>
-      <c r="D39" s="70"/>
-      <c r="E39" s="71"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="56" t="s">
+      <c r="C40" s="70" t="s">
+        <v>275</v>
+      </c>
+      <c r="D40" s="71"/>
+      <c r="E40" s="72"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="56" t="s">
         <v>175</v>
       </c>
-      <c r="B40" s="56" t="s">
+      <c r="B41" s="56" t="s">
         <v>149</v>
       </c>
-      <c r="C40" s="72" t="s">
+      <c r="C41" s="73" t="s">
         <v>152</v>
       </c>
-      <c r="D40" s="73"/>
-      <c r="E40" s="74"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="28" t="s">
+      <c r="D41" s="74"/>
+      <c r="E41" s="75"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="B41" s="28" t="s">
+      <c r="B42" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="C41" s="75" t="s">
+      <c r="C42" s="76" t="s">
         <v>152</v>
       </c>
-      <c r="D41" s="76"/>
-      <c r="E41" s="77"/>
-    </row>
-    <row r="42" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="25" t="s">
+      <c r="D42" s="77"/>
+      <c r="E42" s="78"/>
+    </row>
+    <row r="43" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="25" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="A31:E31"/>
     <mergeCell ref="C39:E39"/>
     <mergeCell ref="C40:E40"/>
     <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C42:E42"/>
     <mergeCell ref="C33:E33"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="C35:E35"/>
     <mergeCell ref="C36:E36"/>
     <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9023,7 +9123,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9037,39 +9137,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="94" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
       <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:5" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="95" t="s">
         <v>251</v>
       </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
       <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="96" t="s">
         <v>225</v>
       </c>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
       <c r="E3" s="15"/>
     </row>
     <row r="4" spans="1:5" ht="380.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="94" t="s">
-        <v>268</v>
-      </c>
-      <c r="B4" s="94"/>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
+      <c r="A4" s="95" t="s">
+        <v>266</v>
+      </c>
+      <c r="B4" s="95"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
       <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9098,7 +9198,7 @@
       </c>
       <c r="C6" s="33"/>
       <c r="D6" s="34" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E6" s="35" t="s">
         <v>222</v>
@@ -9403,189 +9503,197 @@
       <c r="A28" s="61"/>
       <c r="B28" s="39"/>
       <c r="C28" s="39" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D28" s="62" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E28" s="63" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
+    <row r="29" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A29" s="33"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="D29" s="64" t="s">
+        <v>295</v>
+      </c>
+      <c r="E29" s="47" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-    </row>
-    <row r="30" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="94" t="s">
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+    </row>
+    <row r="31" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="95" t="s">
         <v>238</v>
       </c>
-      <c r="B30" s="94"/>
-      <c r="C30" s="94"/>
-      <c r="D30" s="94"/>
-      <c r="E30" s="94"/>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="31" t="s">
+      <c r="B31" s="95"/>
+      <c r="C31" s="95"/>
+      <c r="D31" s="95"/>
+      <c r="E31" s="95"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="31" t="s">
         <v>213</v>
       </c>
-      <c r="B31" s="32" t="s">
+      <c r="B32" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="C31" s="90" t="s">
+      <c r="C32" s="91" t="s">
         <v>204</v>
       </c>
-      <c r="D31" s="91"/>
-      <c r="E31" s="92"/>
-    </row>
-    <row r="32" spans="1:5" ht="217.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="54" t="s">
+      <c r="D32" s="92"/>
+      <c r="E32" s="93"/>
+    </row>
+    <row r="33" spans="1:5" ht="217.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="54" t="s">
         <v>119</v>
       </c>
-      <c r="B32" s="54" t="s">
+      <c r="B33" s="54" t="s">
         <v>214</v>
       </c>
-      <c r="C32" s="78" t="s">
+      <c r="C33" s="79" t="s">
+        <v>267</v>
+      </c>
+      <c r="D33" s="80"/>
+      <c r="E33" s="81"/>
+    </row>
+    <row r="34" spans="1:5" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="C34" s="82" t="s">
         <v>269</v>
       </c>
-      <c r="D32" s="79"/>
-      <c r="E32" s="80"/>
-    </row>
-    <row r="33" spans="1:5" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="B33" s="26" t="s">
-        <v>215</v>
-      </c>
-      <c r="C33" s="81" t="s">
-        <v>271</v>
-      </c>
-      <c r="D33" s="82"/>
-      <c r="E33" s="83"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="55" t="s">
+      <c r="D34" s="83"/>
+      <c r="E34" s="84"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="B34" s="55" t="s">
+      <c r="B35" s="55" t="s">
         <v>216</v>
       </c>
-      <c r="C34" s="84" t="s">
+      <c r="C35" s="85" t="s">
+        <v>270</v>
+      </c>
+      <c r="D35" s="86"/>
+      <c r="E35" s="87"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="C36" s="88" t="s">
+        <v>239</v>
+      </c>
+      <c r="D36" s="89"/>
+      <c r="E36" s="90"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="56" t="s">
+        <v>123</v>
+      </c>
+      <c r="B37" s="57" t="s">
+        <v>218</v>
+      </c>
+      <c r="C37" s="73" t="s">
+        <v>239</v>
+      </c>
+      <c r="D37" s="74"/>
+      <c r="E37" s="75"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B38" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="C38" s="76" t="s">
         <v>272</v>
       </c>
-      <c r="D34" s="85"/>
-      <c r="E34" s="86"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="B35" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="C35" s="87" t="s">
-        <v>239</v>
-      </c>
-      <c r="D35" s="88"/>
-      <c r="E35" s="89"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="56" t="s">
-        <v>123</v>
-      </c>
-      <c r="B36" s="57" t="s">
-        <v>218</v>
-      </c>
-      <c r="C36" s="72" t="s">
-        <v>239</v>
-      </c>
-      <c r="D36" s="73"/>
-      <c r="E36" s="74"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="B37" s="29" t="s">
-        <v>219</v>
-      </c>
-      <c r="C37" s="75" t="s">
-        <v>274</v>
-      </c>
-      <c r="D37" s="76"/>
-      <c r="E37" s="77"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="58" t="s">
+      <c r="D38" s="77"/>
+      <c r="E38" s="78"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="58" t="s">
         <v>173</v>
       </c>
-      <c r="B38" s="58" t="s">
+      <c r="B39" s="58" t="s">
         <v>246</v>
       </c>
-      <c r="C38" s="66" t="s">
+      <c r="C39" s="67" t="s">
         <v>240</v>
       </c>
-      <c r="D38" s="67"/>
-      <c r="E38" s="68"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="29" t="s">
+      <c r="D39" s="68"/>
+      <c r="E39" s="69"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="B39" s="29" t="s">
+      <c r="B40" s="29" t="s">
         <v>245</v>
       </c>
-      <c r="C39" s="69" t="s">
-        <v>275</v>
-      </c>
-      <c r="D39" s="70"/>
-      <c r="E39" s="71"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="56" t="s">
+      <c r="C40" s="70" t="s">
+        <v>273</v>
+      </c>
+      <c r="D40" s="71"/>
+      <c r="E40" s="72"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="56" t="s">
         <v>175</v>
       </c>
-      <c r="B40" s="56" t="s">
+      <c r="B41" s="56" t="s">
         <v>247</v>
       </c>
-      <c r="C40" s="72" t="s">
+      <c r="C41" s="73" t="s">
         <v>240</v>
       </c>
-      <c r="D40" s="73"/>
-      <c r="E40" s="74"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="28" t="s">
+      <c r="D41" s="74"/>
+      <c r="E41" s="75"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="B41" s="28" t="s">
+      <c r="B42" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="C41" s="75" t="s">
+      <c r="C42" s="76" t="s">
         <v>240</v>
       </c>
-      <c r="D41" s="76"/>
-      <c r="E41" s="77"/>
-    </row>
-    <row r="42" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="25" t="s">
+      <c r="D42" s="77"/>
+      <c r="E42" s="78"/>
+    </row>
+    <row r="43" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="25" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:5" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>221</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -9595,22 +9703,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="A31:E31"/>
     <mergeCell ref="C39:E39"/>
     <mergeCell ref="C40:E40"/>
     <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C42:E42"/>
     <mergeCell ref="C33:E33"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="C35:E35"/>
     <mergeCell ref="C36:E36"/>
     <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>